<commit_message>
Se añade la configuración del excel y se obtiene la información de la estación
</commit_message>
<xml_diff>
--- a/src/Controlador/Formatos/registropruebas.xlsx
+++ b/src/Controlador/Formatos/registropruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joseluis.caamal\Documents\GitProjects\SoftwareGasoValidaciones\src\Controlador\Formatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A61363-AD6A-4338-BFCB-425377AEA453}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF2B1287-BA8F-41C1-ACAC-0AA5CD0554C2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
   <si>
     <t>INSTRUMENTOS DE MEDICION GASO, S.A. DE C.V.</t>
   </si>
@@ -465,6 +465,12 @@
   <si>
     <t>DISP</t>
   </si>
+  <si>
+    <t>INICIO</t>
+  </si>
+  <si>
+    <t>FIN</t>
+  </si>
 </sst>
 </file>
 
@@ -474,7 +480,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0000000"/>
   </numFmts>
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -670,6 +676,11 @@
       <b/>
       <sz val="11"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="34">
@@ -1177,7 +1188,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -1282,33 +1293,6 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" wrapText="1"/>
     </xf>
@@ -1345,6 +1329,34 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1703,7 +1715,7 @@
   <dimension ref="A1:BD65"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1824,10 +1836,10 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
-      <c r="T3" s="68" t="s">
+      <c r="T3" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="U3" s="68"/>
+      <c r="U3" s="80"/>
       <c r="AE3" s="4"/>
       <c r="AF3" s="4"/>
       <c r="AG3" s="4"/>
@@ -2324,7 +2336,9 @@
       <c r="BD11" s="4"/>
     </row>
     <row r="12" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
+      <c r="A12" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -2459,10 +2473,10 @@
       <c r="S14" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="T14" s="69" t="s">
+      <c r="T14" s="81" t="s">
         <v>42</v>
       </c>
-      <c r="U14" s="70"/>
+      <c r="U14" s="82"/>
       <c r="V14" s="31" t="s">
         <v>43</v>
       </c>
@@ -2913,6 +2927,9 @@
       <c r="S21" s="7"/>
       <c r="T21" s="7"/>
       <c r="U21" s="8"/>
+      <c r="AC21" s="87" t="s">
+        <v>93</v>
+      </c>
       <c r="AE21" s="4"/>
       <c r="AF21" s="4"/>
       <c r="AG21" s="4"/>
@@ -2941,32 +2958,32 @@
       <c r="BD21" s="4"/>
     </row>
     <row r="22" spans="1:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="71" t="s">
+      <c r="A22" s="83" t="s">
         <v>76</v>
       </c>
-      <c r="B22" s="72"/>
-      <c r="C22" s="72"/>
-      <c r="D22" s="72"/>
-      <c r="E22" s="72"/>
-      <c r="F22" s="72"/>
-      <c r="G22" s="72"/>
-      <c r="H22" s="72"/>
-      <c r="I22" s="72"/>
-      <c r="J22" s="72"/>
-      <c r="K22" s="72"/>
-      <c r="L22" s="72"/>
-      <c r="M22" s="72"/>
-      <c r="N22" s="72"/>
-      <c r="O22" s="72"/>
-      <c r="P22" s="72"/>
-      <c r="Q22" s="72"/>
-      <c r="R22" s="72"/>
-      <c r="S22" s="72"/>
-      <c r="T22" s="72"/>
-      <c r="U22" s="72"/>
-      <c r="V22" s="72"/>
-      <c r="W22" s="72"/>
-      <c r="X22" s="72"/>
+      <c r="B22" s="84"/>
+      <c r="C22" s="84"/>
+      <c r="D22" s="84"/>
+      <c r="E22" s="84"/>
+      <c r="F22" s="84"/>
+      <c r="G22" s="84"/>
+      <c r="H22" s="84"/>
+      <c r="I22" s="84"/>
+      <c r="J22" s="84"/>
+      <c r="K22" s="84"/>
+      <c r="L22" s="84"/>
+      <c r="M22" s="84"/>
+      <c r="N22" s="84"/>
+      <c r="O22" s="84"/>
+      <c r="P22" s="84"/>
+      <c r="Q22" s="84"/>
+      <c r="R22" s="84"/>
+      <c r="S22" s="84"/>
+      <c r="T22" s="84"/>
+      <c r="U22" s="84"/>
+      <c r="V22" s="84"/>
+      <c r="W22" s="84"/>
+      <c r="X22" s="84"/>
       <c r="AE22" s="4"/>
       <c r="AF22" s="4"/>
       <c r="AG22" s="4"/>
@@ -2995,32 +3012,32 @@
       <c r="BD22" s="4"/>
     </row>
     <row r="23" spans="1:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="73" t="s">
+      <c r="A23" s="85" t="s">
         <v>77</v>
       </c>
-      <c r="B23" s="74"/>
-      <c r="C23" s="74"/>
-      <c r="D23" s="74"/>
-      <c r="E23" s="74"/>
-      <c r="F23" s="74"/>
-      <c r="G23" s="74"/>
-      <c r="H23" s="74"/>
-      <c r="I23" s="74"/>
-      <c r="J23" s="74"/>
-      <c r="K23" s="74"/>
-      <c r="L23" s="74"/>
-      <c r="M23" s="74"/>
-      <c r="N23" s="74"/>
-      <c r="O23" s="74"/>
-      <c r="P23" s="74"/>
-      <c r="Q23" s="74"/>
-      <c r="R23" s="74"/>
-      <c r="S23" s="74"/>
-      <c r="T23" s="74"/>
-      <c r="U23" s="74"/>
-      <c r="V23" s="74"/>
-      <c r="W23" s="74"/>
-      <c r="X23" s="74"/>
+      <c r="B23" s="86"/>
+      <c r="C23" s="86"/>
+      <c r="D23" s="86"/>
+      <c r="E23" s="86"/>
+      <c r="F23" s="86"/>
+      <c r="G23" s="86"/>
+      <c r="H23" s="86"/>
+      <c r="I23" s="86"/>
+      <c r="J23" s="86"/>
+      <c r="K23" s="86"/>
+      <c r="L23" s="86"/>
+      <c r="M23" s="86"/>
+      <c r="N23" s="86"/>
+      <c r="O23" s="86"/>
+      <c r="P23" s="86"/>
+      <c r="Q23" s="86"/>
+      <c r="R23" s="86"/>
+      <c r="S23" s="86"/>
+      <c r="T23" s="86"/>
+      <c r="U23" s="86"/>
+      <c r="V23" s="86"/>
+      <c r="W23" s="86"/>
+      <c r="X23" s="86"/>
       <c r="AE23" s="4"/>
       <c r="AF23" s="4"/>
       <c r="AG23" s="4"/>
@@ -3049,32 +3066,32 @@
       <c r="BD23" s="4"/>
     </row>
     <row r="24" spans="1:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="66" t="s">
+      <c r="A24" s="78" t="s">
         <v>78</v>
       </c>
-      <c r="B24" s="67"/>
-      <c r="C24" s="67"/>
-      <c r="D24" s="67"/>
-      <c r="E24" s="67"/>
-      <c r="F24" s="67"/>
-      <c r="G24" s="67"/>
-      <c r="H24" s="67"/>
-      <c r="I24" s="67"/>
-      <c r="J24" s="67"/>
-      <c r="K24" s="67"/>
-      <c r="L24" s="67"/>
-      <c r="M24" s="67"/>
-      <c r="N24" s="67"/>
-      <c r="O24" s="67"/>
-      <c r="P24" s="67"/>
-      <c r="Q24" s="67"/>
-      <c r="R24" s="67"/>
-      <c r="S24" s="67"/>
-      <c r="T24" s="67"/>
-      <c r="U24" s="67"/>
-      <c r="V24" s="67"/>
-      <c r="W24" s="67"/>
-      <c r="X24" s="67"/>
+      <c r="B24" s="79"/>
+      <c r="C24" s="79"/>
+      <c r="D24" s="79"/>
+      <c r="E24" s="79"/>
+      <c r="F24" s="79"/>
+      <c r="G24" s="79"/>
+      <c r="H24" s="79"/>
+      <c r="I24" s="79"/>
+      <c r="J24" s="79"/>
+      <c r="K24" s="79"/>
+      <c r="L24" s="79"/>
+      <c r="M24" s="79"/>
+      <c r="N24" s="79"/>
+      <c r="O24" s="79"/>
+      <c r="P24" s="79"/>
+      <c r="Q24" s="79"/>
+      <c r="R24" s="79"/>
+      <c r="S24" s="79"/>
+      <c r="T24" s="79"/>
+      <c r="U24" s="79"/>
+      <c r="V24" s="79"/>
+      <c r="W24" s="79"/>
+      <c r="X24" s="79"/>
       <c r="AE24" s="4"/>
       <c r="AF24" s="4"/>
       <c r="AG24" s="4"/>
@@ -3103,32 +3120,32 @@
       <c r="BD24" s="4"/>
     </row>
     <row r="25" spans="1:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="66" t="s">
+      <c r="A25" s="78" t="s">
         <v>79</v>
       </c>
-      <c r="B25" s="67"/>
-      <c r="C25" s="67"/>
-      <c r="D25" s="67"/>
-      <c r="E25" s="67"/>
-      <c r="F25" s="67"/>
-      <c r="G25" s="67"/>
-      <c r="H25" s="67"/>
-      <c r="I25" s="67"/>
-      <c r="J25" s="67"/>
-      <c r="K25" s="67"/>
-      <c r="L25" s="67"/>
-      <c r="M25" s="67"/>
-      <c r="N25" s="67"/>
-      <c r="O25" s="67"/>
-      <c r="P25" s="67"/>
-      <c r="Q25" s="67"/>
-      <c r="R25" s="67"/>
-      <c r="S25" s="67"/>
-      <c r="T25" s="67"/>
-      <c r="U25" s="67"/>
-      <c r="V25" s="67"/>
-      <c r="W25" s="67"/>
-      <c r="X25" s="67"/>
+      <c r="B25" s="79"/>
+      <c r="C25" s="79"/>
+      <c r="D25" s="79"/>
+      <c r="E25" s="79"/>
+      <c r="F25" s="79"/>
+      <c r="G25" s="79"/>
+      <c r="H25" s="79"/>
+      <c r="I25" s="79"/>
+      <c r="J25" s="79"/>
+      <c r="K25" s="79"/>
+      <c r="L25" s="79"/>
+      <c r="M25" s="79"/>
+      <c r="N25" s="79"/>
+      <c r="O25" s="79"/>
+      <c r="P25" s="79"/>
+      <c r="Q25" s="79"/>
+      <c r="R25" s="79"/>
+      <c r="S25" s="79"/>
+      <c r="T25" s="79"/>
+      <c r="U25" s="79"/>
+      <c r="V25" s="79"/>
+      <c r="W25" s="79"/>
+      <c r="X25" s="79"/>
       <c r="AE25" s="4"/>
       <c r="AF25" s="4"/>
       <c r="AG25" s="4"/>
@@ -3157,29 +3174,29 @@
       <c r="BD25" s="4"/>
     </row>
     <row r="26" spans="1:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="75" t="s">
+      <c r="A26" s="66" t="s">
         <v>80</v>
       </c>
-      <c r="B26" s="76"/>
-      <c r="C26" s="76"/>
-      <c r="D26" s="76"/>
-      <c r="E26" s="76"/>
-      <c r="F26" s="76"/>
-      <c r="G26" s="76"/>
-      <c r="H26" s="76"/>
-      <c r="I26" s="76"/>
-      <c r="J26" s="76"/>
-      <c r="K26" s="76"/>
-      <c r="L26" s="76"/>
-      <c r="M26" s="76"/>
-      <c r="N26" s="76"/>
-      <c r="O26" s="76"/>
-      <c r="P26" s="76"/>
-      <c r="Q26" s="76"/>
-      <c r="R26" s="76"/>
-      <c r="S26" s="76"/>
-      <c r="T26" s="76"/>
-      <c r="U26" s="77"/>
+      <c r="B26" s="67"/>
+      <c r="C26" s="67"/>
+      <c r="D26" s="67"/>
+      <c r="E26" s="67"/>
+      <c r="F26" s="67"/>
+      <c r="G26" s="67"/>
+      <c r="H26" s="67"/>
+      <c r="I26" s="67"/>
+      <c r="J26" s="67"/>
+      <c r="K26" s="67"/>
+      <c r="L26" s="67"/>
+      <c r="M26" s="67"/>
+      <c r="N26" s="67"/>
+      <c r="O26" s="67"/>
+      <c r="P26" s="67"/>
+      <c r="Q26" s="67"/>
+      <c r="R26" s="67"/>
+      <c r="S26" s="67"/>
+      <c r="T26" s="67"/>
+      <c r="U26" s="68"/>
       <c r="AE26" s="4"/>
       <c r="AF26" s="4"/>
       <c r="AG26" s="4"/>
@@ -3259,20 +3276,20 @@
       <c r="BD27" s="4"/>
     </row>
     <row r="28" spans="1:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="78" t="s">
+      <c r="A28" s="69" t="s">
         <v>82</v>
       </c>
-      <c r="B28" s="79"/>
-      <c r="C28" s="79"/>
-      <c r="D28" s="79"/>
-      <c r="E28" s="79"/>
-      <c r="F28" s="79"/>
-      <c r="G28" s="79"/>
-      <c r="H28" s="79"/>
-      <c r="I28" s="79"/>
-      <c r="J28" s="79"/>
-      <c r="K28" s="79"/>
-      <c r="L28" s="80"/>
+      <c r="B28" s="70"/>
+      <c r="C28" s="70"/>
+      <c r="D28" s="70"/>
+      <c r="E28" s="70"/>
+      <c r="F28" s="70"/>
+      <c r="G28" s="70"/>
+      <c r="H28" s="70"/>
+      <c r="I28" s="70"/>
+      <c r="J28" s="70"/>
+      <c r="K28" s="70"/>
+      <c r="L28" s="71"/>
       <c r="O28" s="60"/>
       <c r="P28" s="60"/>
       <c r="Q28" s="60"/>
@@ -3321,21 +3338,21 @@
       <c r="J29" s="10"/>
       <c r="K29" s="10"/>
       <c r="L29" s="10"/>
-      <c r="M29" s="81" t="s">
+      <c r="M29" s="72" t="s">
         <v>84</v>
       </c>
-      <c r="N29" s="82"/>
-      <c r="O29" s="83"/>
-      <c r="P29" s="84" t="s">
+      <c r="N29" s="73"/>
+      <c r="O29" s="74"/>
+      <c r="P29" s="75" t="s">
         <v>85</v>
       </c>
-      <c r="Q29" s="85"/>
-      <c r="R29" s="86"/>
-      <c r="S29" s="81" t="s">
+      <c r="Q29" s="76"/>
+      <c r="R29" s="77"/>
+      <c r="S29" s="72" t="s">
         <v>86</v>
       </c>
-      <c r="T29" s="82"/>
-      <c r="U29" s="83"/>
+      <c r="T29" s="73"/>
+      <c r="U29" s="74"/>
       <c r="AE29" s="4"/>
       <c r="AF29" s="4"/>
       <c r="AG29" s="4"/>
@@ -4213,17 +4230,17 @@
     <row r="65" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A26:U26"/>
-    <mergeCell ref="A28:L28"/>
-    <mergeCell ref="M29:O29"/>
-    <mergeCell ref="P29:R29"/>
-    <mergeCell ref="S29:U29"/>
     <mergeCell ref="A25:X25"/>
     <mergeCell ref="T3:U3"/>
     <mergeCell ref="T14:U14"/>
     <mergeCell ref="A22:X22"/>
     <mergeCell ref="A23:X23"/>
     <mergeCell ref="A24:X24"/>
+    <mergeCell ref="A26:U26"/>
+    <mergeCell ref="A28:L28"/>
+    <mergeCell ref="M29:O29"/>
+    <mergeCell ref="P29:R29"/>
+    <mergeCell ref="S29:U29"/>
   </mergeCells>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0" footer="0"/>
   <pageSetup scale="43" orientation="landscape" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
Se añade la información del excel para el registro de pruebas
</commit_message>
<xml_diff>
--- a/src/Controlador/Formatos/registropruebas.xlsx
+++ b/src/Controlador/Formatos/registropruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joseluis.caamal\Documents\GitProjects\SoftwareGasoValidaciones\src\Controlador\Formatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF2B1287-BA8F-41C1-ACAC-0AA5CD0554C2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A779B34-6A82-4067-B387-655C9CEAF710}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,14 +18,14 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$A$1:$AC$65</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$A$1:$AA$65</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="110">
   <si>
     <t>INSTRUMENTOS DE MEDICION GASO, S.A. DE C.V.</t>
   </si>
@@ -55,9 +55,6 @@
     <t xml:space="preserve">       Dictamen No. Folio:</t>
   </si>
   <si>
-    <t>Identificacion del elemento primario</t>
-  </si>
-  <si>
     <t>Marca:</t>
   </si>
   <si>
@@ -76,18 +73,9 @@
     <t>Min L/min:</t>
   </si>
   <si>
-    <t>de Medicion</t>
-  </si>
-  <si>
     <t>(alcance de medicion declarado por el fabricante l/min)</t>
   </si>
   <si>
-    <t>Marca:XXXXXXXXXXXXX</t>
-  </si>
-  <si>
-    <t>Modelo:XXXXXXXXXXXXX</t>
-  </si>
-  <si>
     <t>VERIFICACION VISUAL</t>
   </si>
   <si>
@@ -103,9 +91,6 @@
     <t>Signo de pesos en caratula</t>
   </si>
   <si>
-    <t>No. Serie: XXXXXXXXXX</t>
-  </si>
-  <si>
     <t>Dispositivos contador y/o computador:</t>
   </si>
   <si>
@@ -121,9 +106,6 @@
     <t xml:space="preserve">   Tiempo de Corte (80 s) max.</t>
   </si>
   <si>
-    <t>Alcance: XXXXXXXXXXXXX</t>
-  </si>
-  <si>
     <t>Nota:  Indicar con</t>
   </si>
   <si>
@@ -133,9 +115,6 @@
     <t>NC= No cumple</t>
   </si>
   <si>
-    <t>(X) No Aplica</t>
-  </si>
-  <si>
     <t>VERIFICACION METROLOGICA</t>
   </si>
   <si>
@@ -143,12 +122,6 @@
   </si>
   <si>
     <t>LADO:</t>
-  </si>
-  <si>
-    <t>Tot. Inicial:</t>
-  </si>
-  <si>
-    <t>Tot. Final:</t>
   </si>
   <si>
     <t>Resultados:</t>
@@ -436,21 +409,9 @@
     <t>*Lo referente al etiquetado sobre el alcance de medicion solo aplica a dispensarios con aprobacion de modelo y prototipo expedida confome a la NOM-SCFI-005-2011</t>
   </si>
   <si>
-    <t>* Solo aplica a dispensarios con aprobacion de modelo y protitipo expedida conforme a al NOM-SCFI-005-20</t>
-  </si>
-  <si>
-    <t>Errores máximos tolerados y Error de repetibilidad de acuerdo a lo establecido en  la NOM-005-SCFI-2011.</t>
-  </si>
-  <si>
     <t>CLIENTE:</t>
   </si>
   <si>
-    <t>RESPONSABLE DE LA VERIFICACION:</t>
-  </si>
-  <si>
-    <t>TESTIGO:</t>
-  </si>
-  <si>
     <t>-Para aprobación de modelo y prototipo y verificación inicial no debe ser mayor que la suma de (10ml + 2ml por litro).</t>
   </si>
   <si>
@@ -460,16 +421,103 @@
     <t>Nota: Esta prueba se aplica con volúmenes medidos mayores o iguales a 5 veces el volumen mínimo medible (2 litros).</t>
   </si>
   <si>
-    <t>-Para error de repetibilidad que no sea mayor a 20 ml + 2 ml por litro en cualquier gasto (max, med, min).</t>
-  </si>
-  <si>
-    <t>DISP</t>
-  </si>
-  <si>
-    <t>INICIO</t>
-  </si>
-  <si>
-    <t>FIN</t>
+    <t>Numeral Identificacion del elemento primario inciso 7.1.1.2</t>
+  </si>
+  <si>
+    <t>CUMPLE (C)  NO CUMPLE (NC) NO APLICA (NA)</t>
+  </si>
+  <si>
+    <t>Alcance:</t>
+  </si>
+  <si>
+    <t>Aprobación de modelo y prototipo</t>
+  </si>
+  <si>
+    <t>PRECINTO UI:</t>
+  </si>
+  <si>
+    <t>&lt;&lt;DISP&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;MARCA&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;MODELO&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;ESTACION&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;NOSERIE&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;MEDMAX&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;MEDMIN&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;FOLIO&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;DATE&gt;&gt;</t>
+  </si>
+  <si>
+    <t>* Solo aplica a dispensarios con aprobacion de modelo y protitipo expedida conforme a al NOM-SCFI-005-2017</t>
+  </si>
+  <si>
+    <t>Errores máximos tolerados y Error de repetibilidad de acuerdo a lo establecido en  la NOM-005-SCFI-2017.</t>
+  </si>
+  <si>
+    <t>Nota: Para error de repetibilidad que no sea mayor a 20 ml + 2 ml por litro en cualquier gasto (max, med, min).</t>
+  </si>
+  <si>
+    <t>Dispesarios comercializados cuya aprobación de modelo y prototipo bajo la NOM-005-SCFI-2005 estan exentos de este requisito.</t>
+  </si>
+  <si>
+    <t>TECNICO VERIFICADOR</t>
+  </si>
+  <si>
+    <t>PERSONAL DE APOYO</t>
+  </si>
+  <si>
+    <t>Dispensarios comercializados cuya aprobación de modelo y prototipo bajo la NOM-005-SCFI-2011 cumplen con el etiquetado</t>
+  </si>
+  <si>
+    <t>y el gasto cual se realiza la prueba este dentro de la declaración del alcance del elemento primario de medición.</t>
+  </si>
+  <si>
+    <t>Dispensarios comercializados cuya aprobación de modelo o prototipo bajo la NOM-005-SCFI-2017 cumplen con el etiquetado</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> y el alcance del elemento primario de medición y el gasto minimo declarado por el fabricante  no ser mayor a la decima parte del gasto máximo.</t>
+  </si>
+  <si>
+    <t>No Aplica</t>
+  </si>
+  <si>
+    <t>Aplica</t>
+  </si>
+  <si>
+    <t>Cumple</t>
+  </si>
+  <si>
+    <t>NO CUMPLE</t>
+  </si>
+  <si>
+    <t>&lt;&lt;PRODUCTO1&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;LADO1&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;PRECINTO1&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;UVA1&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;PROFECO1&gt;&gt;</t>
   </si>
 </sst>
 </file>
@@ -480,7 +528,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0000000"/>
   </numFmts>
-  <fonts count="32" x14ac:knownFonts="1">
+  <fonts count="34" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -682,8 +730,18 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8.5"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="34">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -869,8 +927,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="24">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -1115,19 +1185,6 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color auto="1"/>
@@ -1188,7 +1245,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -1202,9 +1259,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1226,12 +1280,9 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1239,7 +1290,6 @@
     <xf numFmtId="164" fontId="0" fillId="33" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -1250,19 +1300,16 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1273,36 +1320,82 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="33" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="35" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1311,24 +1404,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1356,7 +1431,27 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="34" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="34" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="34" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1712,35 +1807,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BD65"/>
+  <dimension ref="A1:BB65"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScale="80" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.77734375" customWidth="1"/>
-    <col min="2" max="3" width="7.109375" customWidth="1"/>
+    <col min="2" max="2" width="7.109375" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.33203125" customWidth="1"/>
     <col min="5" max="5" width="11.44140625" customWidth="1"/>
-    <col min="6" max="7" width="6.21875" customWidth="1"/>
+    <col min="6" max="6" width="5.88671875" customWidth="1"/>
+    <col min="7" max="7" width="97.44140625" hidden="1" customWidth="1"/>
     <col min="8" max="9" width="6.44140625" customWidth="1"/>
     <col min="10" max="10" width="8.88671875" customWidth="1"/>
     <col min="11" max="13" width="10.109375" customWidth="1"/>
     <col min="14" max="18" width="11.21875" customWidth="1"/>
-    <col min="19" max="20" width="8.77734375" customWidth="1"/>
-    <col min="21" max="21" width="9.88671875" customWidth="1"/>
-    <col min="22" max="22" width="10.44140625" customWidth="1"/>
-    <col min="23" max="23" width="12.5546875" customWidth="1"/>
+    <col min="19" max="19" width="10.6640625" customWidth="1"/>
+    <col min="20" max="20" width="8.5546875" customWidth="1"/>
+    <col min="21" max="21" width="23.109375" customWidth="1"/>
+    <col min="22" max="22" width="9.33203125" customWidth="1"/>
+    <col min="23" max="23" width="14" customWidth="1"/>
     <col min="24" max="24" width="10.33203125" customWidth="1"/>
     <col min="25" max="25" width="8.33203125" customWidth="1"/>
-    <col min="26" max="33" width="7.33203125" customWidth="1"/>
-    <col min="34" max="34" width="9.44140625" customWidth="1"/>
-    <col min="35" max="256" width="7.33203125" customWidth="1"/>
+    <col min="26" max="31" width="7.33203125" customWidth="1"/>
+    <col min="32" max="32" width="9.44140625" customWidth="1"/>
+    <col min="33" max="254" width="7.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1765,7 +1863,7 @@
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
     </row>
-    <row r="2" spans="1:56" ht="9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1787,6 +1885,8 @@
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
+      <c r="AC2" s="4"/>
+      <c r="AD2" s="4"/>
       <c r="AE2" s="4"/>
       <c r="AF2" s="4"/>
       <c r="AG2" s="4"/>
@@ -1811,10 +1911,8 @@
       <c r="AZ2" s="4"/>
       <c r="BA2" s="4"/>
       <c r="BB2" s="4"/>
-      <c r="BC2" s="4"/>
-      <c r="BD2" s="4"/>
-    </row>
-    <row r="3" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1836,10 +1934,12 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
-      <c r="T3" s="80" t="s">
+      <c r="T3" s="98" t="s">
         <v>2</v>
       </c>
-      <c r="U3" s="80"/>
+      <c r="U3" s="98"/>
+      <c r="AC3" s="4"/>
+      <c r="AD3" s="4"/>
       <c r="AE3" s="4"/>
       <c r="AF3" s="4"/>
       <c r="AG3" s="4"/>
@@ -1864,10 +1964,8 @@
       <c r="AZ3" s="4"/>
       <c r="BA3" s="4"/>
       <c r="BB3" s="4"/>
-      <c r="BC3" s="4"/>
-      <c r="BD3" s="4"/>
-    </row>
-    <row r="4" spans="1:56" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:54" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1878,7 +1976,9 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
+      <c r="K4" s="60" t="s">
+        <v>90</v>
+      </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -1889,6 +1989,8 @@
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
+      <c r="AC4" s="4"/>
+      <c r="AD4" s="4"/>
       <c r="AE4" s="4"/>
       <c r="AF4" s="4"/>
       <c r="AG4" s="4"/>
@@ -1913,22 +2015,22 @@
       <c r="AZ4" s="4"/>
       <c r="BA4" s="4"/>
       <c r="BB4" s="4"/>
-      <c r="BC4" s="4"/>
-      <c r="BD4" s="4"/>
-    </row>
-    <row r="5" spans="1:56" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1"/>
-      <c r="C5" s="7" t="s">
-        <v>91</v>
+      <c r="C5" s="63" t="s">
+        <v>82</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="1"/>
+      <c r="F5" s="64" t="s">
+        <v>85</v>
+      </c>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
       <c r="I5" s="1"/>
@@ -1941,15 +2043,19 @@
         <v>5</v>
       </c>
       <c r="P5" s="1"/>
-      <c r="Q5" s="7"/>
+      <c r="Q5" s="63" t="s">
+        <v>89</v>
+      </c>
       <c r="R5" s="8"/>
-      <c r="S5" s="9"/>
-      <c r="T5" s="10"/>
-      <c r="U5" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="V5" s="10"/>
-      <c r="W5" s="12"/>
+      <c r="S5" s="105" t="s">
+        <v>77</v>
+      </c>
+      <c r="T5" s="106"/>
+      <c r="U5" s="106"/>
+      <c r="V5" s="106"/>
+      <c r="W5" s="107"/>
+      <c r="AC5" s="4"/>
+      <c r="AD5" s="4"/>
       <c r="AE5" s="4"/>
       <c r="AF5" s="4"/>
       <c r="AG5" s="4"/>
@@ -1974,46 +2080,55 @@
       <c r="AZ5" s="4"/>
       <c r="BA5" s="4"/>
       <c r="BB5" s="4"/>
-      <c r="BC5" s="4"/>
-      <c r="BD5" s="4"/>
-    </row>
-    <row r="6" spans="1:56" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="7"/>
+        <v>6</v>
+      </c>
+      <c r="B6" s="63" t="s">
+        <v>83</v>
+      </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
-      <c r="E6" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="7"/>
+      <c r="E6" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="63" t="s">
+        <v>84</v>
+      </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
       <c r="J6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K6" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="K6" s="63" t="s">
+        <v>86</v>
+      </c>
       <c r="L6" s="7"/>
       <c r="M6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N6" s="1"/>
+      <c r="O6" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="N6" s="1"/>
-      <c r="O6" s="14" t="s">
+      <c r="P6" s="63" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q6" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="R6" s="16"/>
-      <c r="S6" s="7"/>
-      <c r="U6" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="V6" s="7"/>
-      <c r="W6" s="8"/>
+      <c r="R6" s="65" t="s">
+        <v>88</v>
+      </c>
+      <c r="S6" s="108"/>
+      <c r="T6" s="109"/>
+      <c r="U6" s="109"/>
+      <c r="V6" s="110"/>
+      <c r="W6" s="111"/>
+      <c r="AC6" s="4"/>
+      <c r="AD6" s="4"/>
       <c r="AE6" s="4"/>
       <c r="AF6" s="4"/>
       <c r="AG6" s="4"/>
@@ -2038,10 +2153,8 @@
       <c r="AZ6" s="4"/>
       <c r="BA6" s="4"/>
       <c r="BB6" s="4"/>
-      <c r="BC6" s="4"/>
-      <c r="BD6" s="4"/>
-    </row>
-    <row r="7" spans="1:56" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -2055,19 +2168,21 @@
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
-      <c r="N7" s="17" t="s">
-        <v>14</v>
+      <c r="N7" s="16" t="s">
+        <v>12</v>
       </c>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
-      <c r="S7" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="T7" s="15"/>
-      <c r="U7" s="15"/>
-      <c r="V7" s="15"/>
-      <c r="W7" s="16"/>
+      <c r="S7" s="57" t="s">
+        <v>6</v>
+      </c>
+      <c r="T7" s="14"/>
+      <c r="U7" s="14"/>
+      <c r="V7" s="14"/>
+      <c r="W7" s="21"/>
+      <c r="AC7" s="4"/>
+      <c r="AD7" s="4"/>
       <c r="AE7" s="4"/>
       <c r="AF7" s="4"/>
       <c r="AG7" s="4"/>
@@ -2092,10 +2207,8 @@
       <c r="AZ7" s="4"/>
       <c r="BA7" s="4"/>
       <c r="BB7" s="4"/>
-      <c r="BC7" s="4"/>
-      <c r="BD7" s="4"/>
-    </row>
-    <row r="8" spans="1:56" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -2114,13 +2227,15 @@
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
-      <c r="S8" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="T8" s="15"/>
-      <c r="U8" s="15"/>
-      <c r="V8" s="15"/>
-      <c r="W8" s="16"/>
+      <c r="S8" s="57" t="s">
+        <v>7</v>
+      </c>
+      <c r="T8" s="14"/>
+      <c r="U8" s="14"/>
+      <c r="V8" s="14"/>
+      <c r="W8" s="21"/>
+      <c r="AC8" s="4"/>
+      <c r="AD8" s="4"/>
       <c r="AE8" s="4"/>
       <c r="AF8" s="4"/>
       <c r="AG8" s="4"/>
@@ -2145,46 +2260,46 @@
       <c r="AZ8" s="4"/>
       <c r="BA8" s="4"/>
       <c r="BB8" s="4"/>
-      <c r="BC8" s="4"/>
-      <c r="BD8" s="4"/>
-    </row>
-    <row r="9" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="21"/>
+    </row>
+    <row r="9" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="19"/>
+      <c r="C9" s="20"/>
       <c r="D9" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="15"/>
+        <v>14</v>
+      </c>
+      <c r="E9" s="14"/>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="23" t="s">
-        <v>19</v>
+      <c r="H9" s="21"/>
+      <c r="I9" s="22" t="s">
+        <v>15</v>
       </c>
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="24" t="s">
-        <v>20</v>
+      <c r="L9" s="21"/>
+      <c r="M9" s="23" t="s">
+        <v>16</v>
       </c>
       <c r="N9" s="10"/>
-      <c r="O9" s="22"/>
-      <c r="P9" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q9" s="22"/>
-      <c r="R9" s="22"/>
-      <c r="S9" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="T9" s="15"/>
+      <c r="O9" s="21"/>
+      <c r="P9" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q9" s="21"/>
+      <c r="R9" s="21"/>
+      <c r="S9" s="57" t="s">
+        <v>8</v>
+      </c>
+      <c r="T9" s="14"/>
       <c r="U9" s="7"/>
-      <c r="V9" s="7"/>
-      <c r="W9" s="8"/>
+      <c r="V9" s="14"/>
+      <c r="W9" s="21"/>
       <c r="X9" s="1"/>
+      <c r="AC9" s="4"/>
+      <c r="AD9" s="4"/>
       <c r="AE9" s="4"/>
       <c r="AF9" s="4"/>
       <c r="AG9" s="4"/>
@@ -2209,45 +2324,45 @@
       <c r="AZ9" s="4"/>
       <c r="BA9" s="4"/>
       <c r="BB9" s="4"/>
-      <c r="BC9" s="4"/>
-      <c r="BD9" s="4"/>
-    </row>
-    <row r="10" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
-        <v>23</v>
+    </row>
+    <row r="10" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A10" s="25" t="s">
+        <v>18</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="27" t="s">
-        <v>24</v>
+      <c r="E10" s="21"/>
+      <c r="F10" s="26" t="s">
+        <v>19</v>
       </c>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="28" t="s">
-        <v>25</v>
+      <c r="I10" s="21"/>
+      <c r="J10" s="27" t="s">
+        <v>20</v>
       </c>
       <c r="K10" s="7"/>
-      <c r="L10" s="22"/>
+      <c r="L10" s="21"/>
       <c r="M10" s="7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="N10" s="7"/>
-      <c r="O10" s="22"/>
-      <c r="P10" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q10" s="22"/>
-      <c r="R10" s="22"/>
-      <c r="S10" s="29" t="s">
-        <v>28</v>
+      <c r="O10" s="21"/>
+      <c r="P10" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q10" s="21"/>
+      <c r="R10" s="21"/>
+      <c r="S10" s="58" t="s">
+        <v>79</v>
       </c>
       <c r="T10" s="1"/>
       <c r="U10" s="7"/>
-      <c r="V10" s="7"/>
-      <c r="W10" s="8"/>
+      <c r="V10" s="14"/>
+      <c r="W10" s="21"/>
+      <c r="AC10" s="4"/>
+      <c r="AD10" s="4"/>
       <c r="AE10" s="4"/>
       <c r="AF10" s="4"/>
       <c r="AG10" s="4"/>
@@ -2272,21 +2387,19 @@
       <c r="AZ10" s="4"/>
       <c r="BA10" s="4"/>
       <c r="BB10" s="4"/>
-      <c r="BC10" s="4"/>
-      <c r="BD10" s="4"/>
-    </row>
-    <row r="11" spans="1:56" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -2300,14 +2413,16 @@
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
-      <c r="S11" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="T11" s="15"/>
+      <c r="S11" s="59" t="s">
+        <v>80</v>
+      </c>
+      <c r="T11" s="14"/>
       <c r="U11" s="7"/>
       <c r="V11" s="7"/>
-      <c r="W11" s="8"/>
+      <c r="W11" s="21"/>
       <c r="X11" s="1"/>
+      <c r="AC11" s="4"/>
+      <c r="AD11" s="4"/>
       <c r="AE11" s="4"/>
       <c r="AF11" s="4"/>
       <c r="AG11" s="4"/>
@@ -2332,13 +2447,9 @@
       <c r="AZ11" s="4"/>
       <c r="BA11" s="4"/>
       <c r="BB11" s="4"/>
-      <c r="BC11" s="4"/>
-      <c r="BD11" s="4"/>
-    </row>
-    <row r="12" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>92</v>
-      </c>
+    </row>
+    <row r="12" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -2356,9 +2467,15 @@
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
-      <c r="S12" s="1"/>
-      <c r="T12" s="1"/>
-      <c r="U12" s="1"/>
+      <c r="S12" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="T12" s="14"/>
+      <c r="U12" s="14"/>
+      <c r="V12" s="7"/>
+      <c r="W12" s="8"/>
+      <c r="AC12" s="4"/>
+      <c r="AD12" s="4"/>
       <c r="AE12" s="4"/>
       <c r="AF12" s="4"/>
       <c r="AG12" s="4"/>
@@ -2383,33 +2500,33 @@
       <c r="AZ12" s="4"/>
       <c r="BA12" s="4"/>
       <c r="BB12" s="4"/>
-      <c r="BC12" s="4"/>
-      <c r="BD12" s="4"/>
-    </row>
-    <row r="13" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="31"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
+    </row>
+    <row r="13" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A13" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="7"/>
       <c r="J13" s="6"/>
-      <c r="K13" s="7"/>
+      <c r="K13" s="1"/>
       <c r="L13" s="6"/>
-      <c r="M13" s="7"/>
+      <c r="M13" s="1"/>
       <c r="N13" s="1"/>
-      <c r="O13" s="7"/>
+      <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
       <c r="U13" s="1"/>
+      <c r="AC13" s="4"/>
+      <c r="AD13" s="4"/>
       <c r="AE13" s="4"/>
       <c r="AF13" s="4"/>
       <c r="AG13" s="4"/>
@@ -2434,61 +2551,65 @@
       <c r="AZ13" s="4"/>
       <c r="BA13" s="4"/>
       <c r="BB13" s="4"/>
-      <c r="BC13" s="4"/>
-      <c r="BD13" s="4"/>
-    </row>
-    <row r="14" spans="1:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="32" t="s">
+    </row>
+    <row r="14" spans="1:54" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="30"/>
+      <c r="C14" s="66" t="s">
+        <v>105</v>
+      </c>
+      <c r="D14" s="19"/>
+      <c r="E14" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="66" t="s">
+        <v>106</v>
+      </c>
+      <c r="G14" s="19"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="62" t="s">
+        <v>81</v>
+      </c>
+      <c r="J14" s="30"/>
+      <c r="K14" s="62" t="s">
+        <v>107</v>
+      </c>
+      <c r="L14" s="30"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="30"/>
+      <c r="P14" s="61" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q14" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="R14" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="S14" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="T14" s="99" t="s">
+        <v>33</v>
+      </c>
+      <c r="U14" s="100"/>
+      <c r="V14" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="33"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="33" t="s">
+      <c r="W14" s="28"/>
+      <c r="X14" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33" t="s">
+      <c r="Y14" s="32"/>
+      <c r="Z14" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="J14" s="33"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="N14" s="20"/>
-      <c r="O14" s="20"/>
-      <c r="P14" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q14" s="35" t="s">
-        <v>39</v>
-      </c>
-      <c r="R14" s="35" t="s">
-        <v>40</v>
-      </c>
-      <c r="S14" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="T14" s="81" t="s">
-        <v>42</v>
-      </c>
-      <c r="U14" s="82"/>
-      <c r="V14" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="W14" s="31"/>
-      <c r="X14" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y14" s="36"/>
-      <c r="Z14" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA14" s="37"/>
+      <c r="AA14" s="33"/>
+      <c r="AC14" s="4"/>
+      <c r="AD14" s="4"/>
       <c r="AE14" s="4"/>
       <c r="AF14" s="4"/>
       <c r="AG14" s="4"/>
@@ -2513,44 +2634,47 @@
       <c r="AZ14" s="4"/>
       <c r="BA14" s="4"/>
       <c r="BB14" s="4"/>
-      <c r="BC14" s="4"/>
-      <c r="BD14" s="4"/>
-    </row>
-    <row r="15" spans="1:56" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="38" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15" s="39"/>
-      <c r="C15" s="39"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="G15" s="39"/>
-      <c r="H15" s="40"/>
-      <c r="I15" s="41"/>
-      <c r="J15" s="41"/>
-      <c r="K15" s="39"/>
-      <c r="L15" s="39"/>
-      <c r="M15" s="39"/>
-      <c r="N15" s="39"/>
-      <c r="O15" s="39"/>
-      <c r="P15" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q15" s="43"/>
-      <c r="R15" s="31"/>
-      <c r="S15" s="44"/>
-      <c r="T15" s="44"/>
-      <c r="U15" s="21"/>
-      <c r="V15" s="44"/>
-      <c r="W15" s="20"/>
-      <c r="X15" s="20"/>
-      <c r="Y15" s="20"/>
-      <c r="Z15" s="20"/>
-      <c r="AA15" s="20"/>
-      <c r="AB15" s="29"/>
+    </row>
+    <row r="15" spans="1:54" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="67" t="s">
+        <v>109</v>
+      </c>
+      <c r="E15" s="36"/>
+      <c r="F15" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" s="35"/>
+      <c r="H15" s="67" t="s">
+        <v>108</v>
+      </c>
+      <c r="I15" s="36"/>
+      <c r="J15" s="36"/>
+      <c r="K15" s="35"/>
+      <c r="L15" s="35"/>
+      <c r="M15" s="35"/>
+      <c r="N15" s="35"/>
+      <c r="O15" s="35"/>
+      <c r="P15" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q15" s="38"/>
+      <c r="R15" s="28"/>
+      <c r="S15" s="39"/>
+      <c r="T15" s="39"/>
+      <c r="U15" s="20"/>
+      <c r="V15" s="39"/>
+      <c r="W15" s="19"/>
+      <c r="X15" s="19"/>
+      <c r="Y15" s="19"/>
+      <c r="Z15" s="19"/>
+      <c r="AA15" s="19"/>
+      <c r="AC15" s="4"/>
+      <c r="AD15" s="4"/>
       <c r="AE15" s="4"/>
       <c r="AF15" s="4"/>
       <c r="AG15" s="4"/>
@@ -2575,84 +2699,83 @@
       <c r="AZ15" s="4"/>
       <c r="BA15" s="4"/>
       <c r="BB15" s="4"/>
-      <c r="BC15" s="4"/>
-      <c r="BD15" s="4"/>
-    </row>
-    <row r="16" spans="1:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="45" t="s">
+    </row>
+    <row r="16" spans="1:54" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="H16" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="I16" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="J16" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="45" t="s">
+      <c r="K16" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="C16" s="45" t="s">
+      <c r="L16" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="45" t="s">
+      <c r="M16" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="E16" s="45" t="s">
+      <c r="N16" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="F16" s="45" t="s">
+      <c r="O16" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="G16" s="45" t="s">
+      <c r="P16" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="H16" s="45" t="s">
+      <c r="Q16" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="I16" s="45" t="s">
+      <c r="R16" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="J16" s="45" t="s">
+      <c r="S16" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="K16" s="45" t="s">
+      <c r="T16" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="L16" s="45" t="s">
+      <c r="U16" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="M16" s="45" t="s">
+      <c r="V16" s="17"/>
+      <c r="W16" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="N16" s="45" t="s">
+      <c r="X16" s="15"/>
+      <c r="Y16" s="17"/>
+      <c r="Z16" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="O16" s="45" t="s">
-        <v>63</v>
-      </c>
-      <c r="P16" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q16" s="45" t="s">
-        <v>65</v>
-      </c>
-      <c r="R16" s="46" t="s">
-        <v>66</v>
-      </c>
-      <c r="S16" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="T16" s="47" t="s">
-        <v>68</v>
-      </c>
-      <c r="U16" s="48" t="s">
-        <v>69</v>
-      </c>
-      <c r="V16" s="18"/>
-      <c r="W16" s="49" t="s">
-        <v>70</v>
-      </c>
-      <c r="X16" s="16"/>
-      <c r="Y16" s="18"/>
-      <c r="Z16" s="50" t="s">
-        <v>71</v>
-      </c>
-      <c r="AA16" s="15"/>
-      <c r="AB16" s="51"/>
+      <c r="AA16" s="14"/>
+      <c r="AC16" s="4"/>
+      <c r="AD16" s="4"/>
       <c r="AE16" s="4"/>
       <c r="AF16" s="4"/>
       <c r="AG16" s="4"/>
@@ -2677,186 +2800,181 @@
       <c r="AZ16" s="4"/>
       <c r="BA16" s="4"/>
       <c r="BB16" s="4"/>
-      <c r="BC16" s="4"/>
-      <c r="BD16" s="4"/>
-    </row>
-    <row r="17" spans="1:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="45" t="s">
-        <v>72</v>
-      </c>
-      <c r="B17" s="45"/>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="45"/>
-      <c r="J17" s="45"/>
-      <c r="K17" s="45"/>
-      <c r="L17" s="45"/>
-      <c r="M17" s="45"/>
-      <c r="N17" s="45"/>
-      <c r="O17" s="45"/>
-      <c r="P17" s="45"/>
-      <c r="Q17" s="45"/>
-      <c r="R17" s="45"/>
-      <c r="S17" s="45"/>
-      <c r="T17" s="45"/>
-      <c r="U17" s="45"/>
-      <c r="V17" s="52"/>
-      <c r="W17" s="52"/>
-      <c r="X17" s="52"/>
-      <c r="Y17" s="52"/>
-      <c r="Z17" s="52"/>
-      <c r="AA17" s="52"/>
-      <c r="AB17" s="53"/>
+    </row>
+    <row r="17" spans="1:54" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="40"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="40"/>
+      <c r="L17" s="40"/>
+      <c r="M17" s="40"/>
+      <c r="N17" s="40"/>
+      <c r="O17" s="40"/>
+      <c r="P17" s="40"/>
+      <c r="Q17" s="40"/>
+      <c r="R17" s="40"/>
+      <c r="S17" s="40"/>
+      <c r="T17" s="40"/>
+      <c r="U17" s="40"/>
+      <c r="V17" s="46"/>
+      <c r="W17" s="46"/>
+      <c r="X17" s="46"/>
+      <c r="Y17" s="46"/>
+      <c r="Z17" s="46"/>
+      <c r="AA17" s="46"/>
+      <c r="AC17" s="4"/>
+      <c r="AD17" s="4"/>
       <c r="AE17" s="4"/>
       <c r="AF17" s="4"/>
       <c r="AG17" s="4"/>
       <c r="AH17" s="4"/>
-      <c r="AI17" s="4"/>
-      <c r="AJ17" s="4"/>
-      <c r="AK17" s="54"/>
-      <c r="AL17" s="54"/>
-      <c r="AM17" s="55"/>
-      <c r="AN17" s="55"/>
-      <c r="AO17" s="55"/>
-      <c r="AP17" s="55"/>
-      <c r="AQ17" s="55"/>
-      <c r="AR17" s="55"/>
-      <c r="AS17" s="55"/>
-      <c r="AT17" s="55"/>
-      <c r="AU17" s="4"/>
-      <c r="AV17" s="54"/>
-      <c r="AW17" s="54"/>
-      <c r="AX17" s="55"/>
-      <c r="AY17" s="55"/>
-      <c r="AZ17" s="55"/>
-      <c r="BA17" s="55"/>
-      <c r="BB17" s="55"/>
-      <c r="BC17" s="55"/>
-      <c r="BD17" s="4"/>
-    </row>
-    <row r="18" spans="1:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="45" t="s">
-        <v>73</v>
-      </c>
-      <c r="B18" s="45"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="45"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="45"/>
-      <c r="I18" s="45"/>
-      <c r="J18" s="45"/>
-      <c r="K18" s="45"/>
-      <c r="L18" s="45"/>
-      <c r="M18" s="45"/>
-      <c r="N18" s="45"/>
-      <c r="O18" s="45"/>
-      <c r="P18" s="45"/>
-      <c r="Q18" s="45"/>
-      <c r="R18" s="45"/>
-      <c r="S18" s="45"/>
-      <c r="T18" s="45"/>
-      <c r="U18" s="45"/>
-      <c r="V18" s="52"/>
-      <c r="W18" s="52"/>
-      <c r="X18" s="52"/>
-      <c r="Y18" s="52"/>
-      <c r="Z18" s="52"/>
-      <c r="AA18" s="52"/>
-      <c r="AB18" s="53"/>
+      <c r="AI17" s="48"/>
+      <c r="AJ17" s="48"/>
+      <c r="AK17" s="49"/>
+      <c r="AL17" s="49"/>
+      <c r="AM17" s="49"/>
+      <c r="AN17" s="49"/>
+      <c r="AO17" s="49"/>
+      <c r="AP17" s="49"/>
+      <c r="AQ17" s="49"/>
+      <c r="AR17" s="49"/>
+      <c r="AS17" s="4"/>
+      <c r="AT17" s="48"/>
+      <c r="AU17" s="48"/>
+      <c r="AV17" s="49"/>
+      <c r="AW17" s="49"/>
+      <c r="AX17" s="49"/>
+      <c r="AY17" s="49"/>
+      <c r="AZ17" s="49"/>
+      <c r="BA17" s="49"/>
+      <c r="BB17" s="4"/>
+    </row>
+    <row r="18" spans="1:54" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
+      <c r="K18" s="40"/>
+      <c r="L18" s="40"/>
+      <c r="M18" s="40"/>
+      <c r="N18" s="40"/>
+      <c r="O18" s="40"/>
+      <c r="P18" s="40"/>
+      <c r="Q18" s="40"/>
+      <c r="R18" s="40"/>
+      <c r="S18" s="40"/>
+      <c r="T18" s="40"/>
+      <c r="U18" s="40"/>
+      <c r="V18" s="46"/>
+      <c r="W18" s="46"/>
+      <c r="X18" s="46"/>
+      <c r="Y18" s="46"/>
+      <c r="Z18" s="46"/>
+      <c r="AA18" s="46"/>
+      <c r="AC18" s="4"/>
+      <c r="AD18" s="4"/>
       <c r="AE18" s="4"/>
       <c r="AF18" s="4"/>
       <c r="AG18" s="4"/>
-      <c r="AH18" s="4"/>
-      <c r="AI18" s="4"/>
-      <c r="AJ18" s="56"/>
-      <c r="AK18" s="54"/>
-      <c r="AL18" s="54"/>
-      <c r="AM18" s="55"/>
-      <c r="AN18" s="55"/>
-      <c r="AO18" s="55"/>
-      <c r="AP18" s="55"/>
-      <c r="AQ18" s="55"/>
-      <c r="AR18" s="55"/>
-      <c r="AS18" s="55"/>
-      <c r="AT18" s="55"/>
-      <c r="AU18" s="56"/>
-      <c r="AV18" s="54"/>
-      <c r="AW18" s="54"/>
-      <c r="AX18" s="55"/>
-      <c r="AY18" s="55"/>
-      <c r="AZ18" s="55"/>
-      <c r="BA18" s="55"/>
-      <c r="BB18" s="55"/>
-      <c r="BC18" s="55"/>
-      <c r="BD18" s="4"/>
-    </row>
-    <row r="19" spans="1:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="45" t="s">
-        <v>74</v>
-      </c>
-      <c r="B19" s="45"/>
-      <c r="C19" s="45"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="45"/>
-      <c r="G19" s="45"/>
-      <c r="H19" s="45"/>
-      <c r="I19" s="45"/>
-      <c r="J19" s="45"/>
-      <c r="K19" s="45"/>
-      <c r="L19" s="45"/>
-      <c r="M19" s="45"/>
-      <c r="N19" s="45"/>
-      <c r="O19" s="45"/>
-      <c r="P19" s="45"/>
-      <c r="Q19" s="45"/>
-      <c r="R19" s="45"/>
-      <c r="S19" s="45"/>
-      <c r="T19" s="45"/>
-      <c r="U19" s="45"/>
-      <c r="V19" s="52"/>
-      <c r="W19" s="52"/>
-      <c r="X19" s="52"/>
-      <c r="Y19" s="52"/>
-      <c r="Z19" s="52"/>
-      <c r="AA19" s="52"/>
-      <c r="AB19" s="53"/>
+      <c r="AH18" s="50"/>
+      <c r="AI18" s="48"/>
+      <c r="AJ18" s="48"/>
+      <c r="AK18" s="49"/>
+      <c r="AL18" s="49"/>
+      <c r="AM18" s="49"/>
+      <c r="AN18" s="49"/>
+      <c r="AO18" s="49"/>
+      <c r="AP18" s="49"/>
+      <c r="AQ18" s="49"/>
+      <c r="AR18" s="49"/>
+      <c r="AS18" s="50"/>
+      <c r="AT18" s="48"/>
+      <c r="AU18" s="48"/>
+      <c r="AV18" s="49"/>
+      <c r="AW18" s="49"/>
+      <c r="AX18" s="49"/>
+      <c r="AY18" s="49"/>
+      <c r="AZ18" s="49"/>
+      <c r="BA18" s="49"/>
+      <c r="BB18" s="4"/>
+    </row>
+    <row r="19" spans="1:54" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="40"/>
+      <c r="K19" s="40"/>
+      <c r="L19" s="40"/>
+      <c r="M19" s="40"/>
+      <c r="N19" s="40"/>
+      <c r="O19" s="40"/>
+      <c r="P19" s="40"/>
+      <c r="Q19" s="40"/>
+      <c r="R19" s="40"/>
+      <c r="S19" s="40"/>
+      <c r="T19" s="40"/>
+      <c r="U19" s="40"/>
+      <c r="V19" s="46"/>
+      <c r="W19" s="46"/>
+      <c r="X19" s="46"/>
+      <c r="Y19" s="46"/>
+      <c r="Z19" s="46"/>
+      <c r="AA19" s="46"/>
+      <c r="AC19" s="4"/>
+      <c r="AD19" s="4"/>
       <c r="AE19" s="4"/>
       <c r="AF19" s="4"/>
       <c r="AG19" s="4"/>
-      <c r="AH19" s="4"/>
-      <c r="AI19" s="4"/>
-      <c r="AJ19" s="54"/>
-      <c r="AK19" s="54"/>
-      <c r="AL19" s="54"/>
-      <c r="AM19" s="55"/>
-      <c r="AN19" s="55"/>
-      <c r="AO19" s="55"/>
-      <c r="AP19" s="55"/>
-      <c r="AQ19" s="55"/>
-      <c r="AR19" s="55"/>
-      <c r="AS19" s="55"/>
-      <c r="AT19" s="55"/>
-      <c r="AU19" s="54"/>
-      <c r="AV19" s="54"/>
-      <c r="AW19" s="54"/>
-      <c r="AX19" s="55"/>
-      <c r="AY19" s="55"/>
-      <c r="AZ19" s="55"/>
-      <c r="BA19" s="55"/>
-      <c r="BB19" s="55"/>
-      <c r="BC19" s="55"/>
-      <c r="BD19" s="4"/>
-    </row>
-    <row r="20" spans="1:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH19" s="48"/>
+      <c r="AI19" s="48"/>
+      <c r="AJ19" s="48"/>
+      <c r="AK19" s="49"/>
+      <c r="AL19" s="49"/>
+      <c r="AM19" s="49"/>
+      <c r="AN19" s="49"/>
+      <c r="AO19" s="49"/>
+      <c r="AP19" s="49"/>
+      <c r="AQ19" s="49"/>
+      <c r="AR19" s="49"/>
+      <c r="AS19" s="48"/>
+      <c r="AT19" s="48"/>
+      <c r="AU19" s="48"/>
+      <c r="AV19" s="49"/>
+      <c r="AW19" s="49"/>
+      <c r="AX19" s="49"/>
+      <c r="AY19" s="49"/>
+      <c r="AZ19" s="49"/>
+      <c r="BA19" s="49"/>
+      <c r="BB19" s="4"/>
+    </row>
+    <row r="20" spans="1:54" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
@@ -2877,36 +2995,36 @@
       <c r="R20" s="10"/>
       <c r="S20" s="10"/>
       <c r="T20" s="10"/>
-      <c r="U20" s="12"/>
+      <c r="U20" s="11"/>
+      <c r="AC20" s="4"/>
+      <c r="AD20" s="4"/>
       <c r="AE20" s="4"/>
       <c r="AF20" s="4"/>
       <c r="AG20" s="4"/>
       <c r="AH20" s="4"/>
-      <c r="AI20" s="4"/>
-      <c r="AJ20" s="4"/>
-      <c r="AK20" s="54"/>
-      <c r="AL20" s="54"/>
-      <c r="AM20" s="55"/>
-      <c r="AN20" s="55"/>
-      <c r="AO20" s="55"/>
-      <c r="AP20" s="55"/>
-      <c r="AQ20" s="55"/>
-      <c r="AR20" s="55"/>
-      <c r="AS20" s="55"/>
-      <c r="AT20" s="55"/>
-      <c r="AU20" s="4"/>
-      <c r="AV20" s="54"/>
-      <c r="AW20" s="54"/>
-      <c r="AX20" s="55"/>
-      <c r="AY20" s="55"/>
-      <c r="AZ20" s="55"/>
-      <c r="BA20" s="55"/>
-      <c r="BB20" s="55"/>
-      <c r="BC20" s="55"/>
-      <c r="BD20" s="4"/>
-    </row>
-    <row r="21" spans="1:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="57"/>
+      <c r="AI20" s="48"/>
+      <c r="AJ20" s="48"/>
+      <c r="AK20" s="49"/>
+      <c r="AL20" s="49"/>
+      <c r="AM20" s="49"/>
+      <c r="AN20" s="49"/>
+      <c r="AO20" s="49"/>
+      <c r="AP20" s="49"/>
+      <c r="AQ20" s="49"/>
+      <c r="AR20" s="49"/>
+      <c r="AS20" s="4"/>
+      <c r="AT20" s="48"/>
+      <c r="AU20" s="48"/>
+      <c r="AV20" s="49"/>
+      <c r="AW20" s="49"/>
+      <c r="AX20" s="49"/>
+      <c r="AY20" s="49"/>
+      <c r="AZ20" s="49"/>
+      <c r="BA20" s="49"/>
+      <c r="BB20" s="4"/>
+    </row>
+    <row r="21" spans="1:54" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="51"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -2927,376 +3045,387 @@
       <c r="S21" s="7"/>
       <c r="T21" s="7"/>
       <c r="U21" s="8"/>
-      <c r="AC21" s="87" t="s">
-        <v>93</v>
-      </c>
+      <c r="AC21" s="4"/>
+      <c r="AD21" s="4"/>
       <c r="AE21" s="4"/>
       <c r="AF21" s="4"/>
       <c r="AG21" s="4"/>
       <c r="AH21" s="4"/>
-      <c r="AI21" s="4"/>
-      <c r="AJ21" s="4"/>
-      <c r="AK21" s="54"/>
-      <c r="AL21" s="54"/>
-      <c r="AM21" s="55"/>
-      <c r="AN21" s="55"/>
-      <c r="AO21" s="55"/>
-      <c r="AP21" s="55"/>
-      <c r="AQ21" s="55"/>
-      <c r="AR21" s="55"/>
-      <c r="AS21" s="55"/>
-      <c r="AT21" s="55"/>
-      <c r="AU21" s="4"/>
-      <c r="AV21" s="54"/>
-      <c r="AW21" s="54"/>
-      <c r="AX21" s="55"/>
-      <c r="AY21" s="55"/>
-      <c r="AZ21" s="55"/>
-      <c r="BA21" s="55"/>
-      <c r="BB21" s="55"/>
-      <c r="BC21" s="55"/>
-      <c r="BD21" s="4"/>
-    </row>
-    <row r="22" spans="1:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="83" t="s">
-        <v>76</v>
-      </c>
-      <c r="B22" s="84"/>
-      <c r="C22" s="84"/>
-      <c r="D22" s="84"/>
-      <c r="E22" s="84"/>
-      <c r="F22" s="84"/>
-      <c r="G22" s="84"/>
-      <c r="H22" s="84"/>
-      <c r="I22" s="84"/>
-      <c r="J22" s="84"/>
-      <c r="K22" s="84"/>
-      <c r="L22" s="84"/>
-      <c r="M22" s="84"/>
-      <c r="N22" s="84"/>
-      <c r="O22" s="84"/>
-      <c r="P22" s="84"/>
-      <c r="Q22" s="84"/>
-      <c r="R22" s="84"/>
-      <c r="S22" s="84"/>
-      <c r="T22" s="84"/>
-      <c r="U22" s="84"/>
-      <c r="V22" s="84"/>
-      <c r="W22" s="84"/>
-      <c r="X22" s="84"/>
+      <c r="AI21" s="48"/>
+      <c r="AJ21" s="48"/>
+      <c r="AK21" s="49"/>
+      <c r="AL21" s="49"/>
+      <c r="AM21" s="49"/>
+      <c r="AN21" s="49"/>
+      <c r="AO21" s="49"/>
+      <c r="AP21" s="49"/>
+      <c r="AQ21" s="49"/>
+      <c r="AR21" s="49"/>
+      <c r="AS21" s="4"/>
+      <c r="AT21" s="48"/>
+      <c r="AU21" s="48"/>
+      <c r="AV21" s="49"/>
+      <c r="AW21" s="49"/>
+      <c r="AX21" s="49"/>
+      <c r="AY21" s="49"/>
+      <c r="AZ21" s="49"/>
+      <c r="BA21" s="49"/>
+      <c r="BB21" s="4"/>
+    </row>
+    <row r="22" spans="1:54" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="101" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="102"/>
+      <c r="C22" s="102"/>
+      <c r="D22" s="102"/>
+      <c r="E22" s="102"/>
+      <c r="F22" s="102"/>
+      <c r="G22" s="102"/>
+      <c r="H22" s="102"/>
+      <c r="I22" s="102"/>
+      <c r="J22" s="102"/>
+      <c r="K22" s="102"/>
+      <c r="L22" s="102"/>
+      <c r="M22" s="102"/>
+      <c r="N22" s="102"/>
+      <c r="O22" s="102"/>
+      <c r="P22" s="102"/>
+      <c r="Q22" s="102"/>
+      <c r="R22" s="102"/>
+      <c r="S22" s="102"/>
+      <c r="T22" s="102"/>
+      <c r="U22" s="102"/>
+      <c r="V22" s="102"/>
+      <c r="W22" s="102"/>
+      <c r="X22" s="102"/>
+      <c r="AC22" s="4"/>
+      <c r="AD22" s="4"/>
       <c r="AE22" s="4"/>
       <c r="AF22" s="4"/>
       <c r="AG22" s="4"/>
-      <c r="AH22" s="4"/>
-      <c r="AI22" s="4"/>
-      <c r="AJ22" s="56"/>
-      <c r="AK22" s="54"/>
-      <c r="AL22" s="54"/>
-      <c r="AM22" s="55"/>
-      <c r="AN22" s="55"/>
-      <c r="AO22" s="55"/>
-      <c r="AP22" s="55"/>
-      <c r="AQ22" s="55"/>
-      <c r="AR22" s="55"/>
-      <c r="AS22" s="55"/>
-      <c r="AT22" s="55"/>
-      <c r="AU22" s="56"/>
-      <c r="AV22" s="54"/>
-      <c r="AW22" s="54"/>
-      <c r="AX22" s="55"/>
-      <c r="AY22" s="55"/>
-      <c r="AZ22" s="55"/>
-      <c r="BA22" s="55"/>
-      <c r="BB22" s="55"/>
-      <c r="BC22" s="55"/>
-      <c r="BD22" s="4"/>
-    </row>
-    <row r="23" spans="1:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="85" t="s">
-        <v>77</v>
-      </c>
-      <c r="B23" s="86"/>
-      <c r="C23" s="86"/>
-      <c r="D23" s="86"/>
-      <c r="E23" s="86"/>
-      <c r="F23" s="86"/>
-      <c r="G23" s="86"/>
-      <c r="H23" s="86"/>
-      <c r="I23" s="86"/>
-      <c r="J23" s="86"/>
-      <c r="K23" s="86"/>
-      <c r="L23" s="86"/>
-      <c r="M23" s="86"/>
-      <c r="N23" s="86"/>
-      <c r="O23" s="86"/>
-      <c r="P23" s="86"/>
-      <c r="Q23" s="86"/>
-      <c r="R23" s="86"/>
-      <c r="S23" s="86"/>
-      <c r="T23" s="86"/>
-      <c r="U23" s="86"/>
-      <c r="V23" s="86"/>
-      <c r="W23" s="86"/>
-      <c r="X23" s="86"/>
+      <c r="AH22" s="50"/>
+      <c r="AI22" s="48"/>
+      <c r="AJ22" s="48"/>
+      <c r="AK22" s="49"/>
+      <c r="AL22" s="49"/>
+      <c r="AM22" s="49"/>
+      <c r="AN22" s="49"/>
+      <c r="AO22" s="49"/>
+      <c r="AP22" s="49"/>
+      <c r="AQ22" s="49"/>
+      <c r="AR22" s="49"/>
+      <c r="AS22" s="50"/>
+      <c r="AT22" s="48"/>
+      <c r="AU22" s="48"/>
+      <c r="AV22" s="49"/>
+      <c r="AW22" s="49"/>
+      <c r="AX22" s="49"/>
+      <c r="AY22" s="49"/>
+      <c r="AZ22" s="49"/>
+      <c r="BA22" s="49"/>
+      <c r="BB22" s="4"/>
+    </row>
+    <row r="23" spans="1:54" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="103" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" s="104"/>
+      <c r="C23" s="104"/>
+      <c r="D23" s="104"/>
+      <c r="E23" s="104"/>
+      <c r="F23" s="104"/>
+      <c r="G23" s="104"/>
+      <c r="H23" s="104"/>
+      <c r="I23" s="104"/>
+      <c r="J23" s="104"/>
+      <c r="K23" s="104"/>
+      <c r="L23" s="104"/>
+      <c r="M23" s="104"/>
+      <c r="N23" s="104"/>
+      <c r="O23" s="104"/>
+      <c r="P23" s="104"/>
+      <c r="Q23" s="104"/>
+      <c r="R23" s="104"/>
+      <c r="S23" s="104"/>
+      <c r="T23" s="104"/>
+      <c r="U23" s="104"/>
+      <c r="V23" s="104"/>
+      <c r="W23" s="104"/>
+      <c r="X23" s="104"/>
+      <c r="AC23" s="4"/>
+      <c r="AD23" s="4"/>
       <c r="AE23" s="4"/>
       <c r="AF23" s="4"/>
       <c r="AG23" s="4"/>
       <c r="AH23" s="4"/>
-      <c r="AI23" s="4"/>
-      <c r="AJ23" s="4"/>
-      <c r="AK23" s="54"/>
-      <c r="AL23" s="54"/>
-      <c r="AM23" s="55"/>
-      <c r="AN23" s="55"/>
-      <c r="AO23" s="55"/>
-      <c r="AP23" s="55"/>
-      <c r="AQ23" s="55"/>
-      <c r="AR23" s="55"/>
-      <c r="AS23" s="55"/>
-      <c r="AT23" s="55"/>
-      <c r="AU23" s="4"/>
-      <c r="AV23" s="54"/>
-      <c r="AW23" s="54"/>
-      <c r="AX23" s="55"/>
-      <c r="AY23" s="55"/>
-      <c r="AZ23" s="55"/>
-      <c r="BA23" s="55"/>
-      <c r="BB23" s="55"/>
-      <c r="BC23" s="55"/>
-      <c r="BD23" s="4"/>
-    </row>
-    <row r="24" spans="1:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="78" t="s">
-        <v>78</v>
-      </c>
-      <c r="B24" s="79"/>
-      <c r="C24" s="79"/>
-      <c r="D24" s="79"/>
-      <c r="E24" s="79"/>
-      <c r="F24" s="79"/>
-      <c r="G24" s="79"/>
-      <c r="H24" s="79"/>
-      <c r="I24" s="79"/>
-      <c r="J24" s="79"/>
-      <c r="K24" s="79"/>
-      <c r="L24" s="79"/>
-      <c r="M24" s="79"/>
-      <c r="N24" s="79"/>
-      <c r="O24" s="79"/>
-      <c r="P24" s="79"/>
-      <c r="Q24" s="79"/>
-      <c r="R24" s="79"/>
-      <c r="S24" s="79"/>
-      <c r="T24" s="79"/>
-      <c r="U24" s="79"/>
-      <c r="V24" s="79"/>
-      <c r="W24" s="79"/>
-      <c r="X24" s="79"/>
+      <c r="AI23" s="48"/>
+      <c r="AJ23" s="48"/>
+      <c r="AK23" s="49"/>
+      <c r="AL23" s="49"/>
+      <c r="AM23" s="49"/>
+      <c r="AN23" s="49"/>
+      <c r="AO23" s="49"/>
+      <c r="AP23" s="49"/>
+      <c r="AQ23" s="49"/>
+      <c r="AR23" s="49"/>
+      <c r="AS23" s="4"/>
+      <c r="AT23" s="48"/>
+      <c r="AU23" s="48"/>
+      <c r="AV23" s="49"/>
+      <c r="AW23" s="49"/>
+      <c r="AX23" s="49"/>
+      <c r="AY23" s="49"/>
+      <c r="AZ23" s="49"/>
+      <c r="BA23" s="49"/>
+      <c r="BB23" s="4"/>
+    </row>
+    <row r="24" spans="1:54" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="96" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" s="97"/>
+      <c r="C24" s="97"/>
+      <c r="D24" s="97"/>
+      <c r="E24" s="97"/>
+      <c r="F24" s="97"/>
+      <c r="G24" s="97"/>
+      <c r="H24" s="97"/>
+      <c r="I24" s="97"/>
+      <c r="J24" s="97"/>
+      <c r="K24" s="97"/>
+      <c r="L24" s="97"/>
+      <c r="M24" s="97"/>
+      <c r="N24" s="97"/>
+      <c r="O24" s="97"/>
+      <c r="P24" s="97"/>
+      <c r="Q24" s="97"/>
+      <c r="R24" s="97"/>
+      <c r="S24" s="97"/>
+      <c r="T24" s="97"/>
+      <c r="U24" s="97"/>
+      <c r="V24" s="97"/>
+      <c r="W24" s="97"/>
+      <c r="X24" s="97"/>
+      <c r="AC24" s="4"/>
+      <c r="AD24" s="4"/>
       <c r="AE24" s="4"/>
       <c r="AF24" s="4"/>
       <c r="AG24" s="4"/>
       <c r="AH24" s="4"/>
-      <c r="AI24" s="4"/>
-      <c r="AJ24" s="4"/>
-      <c r="AK24" s="54"/>
-      <c r="AL24" s="54"/>
-      <c r="AM24" s="55"/>
-      <c r="AN24" s="55"/>
-      <c r="AO24" s="55"/>
-      <c r="AP24" s="55"/>
-      <c r="AQ24" s="55"/>
-      <c r="AR24" s="55"/>
-      <c r="AS24" s="55"/>
-      <c r="AT24" s="55"/>
-      <c r="AU24" s="4"/>
-      <c r="AV24" s="54"/>
-      <c r="AW24" s="54"/>
-      <c r="AX24" s="55"/>
-      <c r="AY24" s="55"/>
-      <c r="AZ24" s="55"/>
-      <c r="BA24" s="55"/>
-      <c r="BB24" s="55"/>
-      <c r="BC24" s="55"/>
-      <c r="BD24" s="4"/>
-    </row>
-    <row r="25" spans="1:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="78" t="s">
-        <v>79</v>
-      </c>
-      <c r="B25" s="79"/>
-      <c r="C25" s="79"/>
-      <c r="D25" s="79"/>
-      <c r="E25" s="79"/>
-      <c r="F25" s="79"/>
-      <c r="G25" s="79"/>
-      <c r="H25" s="79"/>
-      <c r="I25" s="79"/>
-      <c r="J25" s="79"/>
-      <c r="K25" s="79"/>
-      <c r="L25" s="79"/>
-      <c r="M25" s="79"/>
-      <c r="N25" s="79"/>
-      <c r="O25" s="79"/>
-      <c r="P25" s="79"/>
-      <c r="Q25" s="79"/>
-      <c r="R25" s="79"/>
-      <c r="S25" s="79"/>
-      <c r="T25" s="79"/>
-      <c r="U25" s="79"/>
-      <c r="V25" s="79"/>
-      <c r="W25" s="79"/>
-      <c r="X25" s="79"/>
+      <c r="AI24" s="48"/>
+      <c r="AJ24" s="48"/>
+      <c r="AK24" s="49"/>
+      <c r="AL24" s="49"/>
+      <c r="AM24" s="49"/>
+      <c r="AN24" s="49"/>
+      <c r="AO24" s="49"/>
+      <c r="AP24" s="49"/>
+      <c r="AQ24" s="49"/>
+      <c r="AR24" s="49"/>
+      <c r="AS24" s="4"/>
+      <c r="AT24" s="48"/>
+      <c r="AU24" s="48"/>
+      <c r="AV24" s="49"/>
+      <c r="AW24" s="49"/>
+      <c r="AX24" s="49"/>
+      <c r="AY24" s="49"/>
+      <c r="AZ24" s="49"/>
+      <c r="BA24" s="49"/>
+      <c r="BB24" s="4"/>
+    </row>
+    <row r="25" spans="1:54" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="96" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="97"/>
+      <c r="C25" s="97"/>
+      <c r="D25" s="97"/>
+      <c r="E25" s="97"/>
+      <c r="F25" s="97"/>
+      <c r="G25" s="97"/>
+      <c r="H25" s="97"/>
+      <c r="I25" s="97"/>
+      <c r="J25" s="97"/>
+      <c r="K25" s="97"/>
+      <c r="L25" s="97"/>
+      <c r="M25" s="97"/>
+      <c r="N25" s="97"/>
+      <c r="O25" s="97"/>
+      <c r="P25" s="97"/>
+      <c r="Q25" s="97"/>
+      <c r="R25" s="97"/>
+      <c r="S25" s="97"/>
+      <c r="T25" s="97"/>
+      <c r="U25" s="97"/>
+      <c r="V25" s="97"/>
+      <c r="W25" s="97"/>
+      <c r="X25" s="97"/>
+      <c r="AC25" s="4"/>
+      <c r="AD25" s="4"/>
       <c r="AE25" s="4"/>
       <c r="AF25" s="4"/>
       <c r="AG25" s="4"/>
-      <c r="AH25" s="4"/>
-      <c r="AI25" s="4"/>
-      <c r="AJ25" s="54"/>
-      <c r="AK25" s="54"/>
-      <c r="AL25" s="54"/>
-      <c r="AM25" s="55"/>
-      <c r="AN25" s="55"/>
-      <c r="AO25" s="55"/>
-      <c r="AP25" s="55"/>
-      <c r="AQ25" s="55"/>
-      <c r="AR25" s="55"/>
-      <c r="AS25" s="55"/>
-      <c r="AT25" s="55"/>
-      <c r="AU25" s="54"/>
-      <c r="AV25" s="54"/>
-      <c r="AW25" s="54"/>
-      <c r="AX25" s="55"/>
-      <c r="AY25" s="55"/>
-      <c r="AZ25" s="55"/>
-      <c r="BA25" s="55"/>
-      <c r="BB25" s="55"/>
-      <c r="BC25" s="55"/>
-      <c r="BD25" s="4"/>
-    </row>
-    <row r="26" spans="1:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="66" t="s">
-        <v>80</v>
-      </c>
-      <c r="B26" s="67"/>
-      <c r="C26" s="67"/>
-      <c r="D26" s="67"/>
-      <c r="E26" s="67"/>
-      <c r="F26" s="67"/>
-      <c r="G26" s="67"/>
-      <c r="H26" s="67"/>
-      <c r="I26" s="67"/>
-      <c r="J26" s="67"/>
-      <c r="K26" s="67"/>
-      <c r="L26" s="67"/>
-      <c r="M26" s="67"/>
-      <c r="N26" s="67"/>
-      <c r="O26" s="67"/>
-      <c r="P26" s="67"/>
-      <c r="Q26" s="67"/>
-      <c r="R26" s="67"/>
-      <c r="S26" s="67"/>
-      <c r="T26" s="67"/>
-      <c r="U26" s="68"/>
+      <c r="AH25" s="48"/>
+      <c r="AI25" s="48"/>
+      <c r="AJ25" s="48"/>
+      <c r="AK25" s="49"/>
+      <c r="AL25" s="49"/>
+      <c r="AM25" s="49"/>
+      <c r="AN25" s="49"/>
+      <c r="AO25" s="49"/>
+      <c r="AP25" s="49"/>
+      <c r="AQ25" s="49"/>
+      <c r="AR25" s="49"/>
+      <c r="AS25" s="48"/>
+      <c r="AT25" s="48"/>
+      <c r="AU25" s="48"/>
+      <c r="AV25" s="49"/>
+      <c r="AW25" s="49"/>
+      <c r="AX25" s="49"/>
+      <c r="AY25" s="49"/>
+      <c r="AZ25" s="49"/>
+      <c r="BA25" s="49"/>
+      <c r="BB25" s="4"/>
+    </row>
+    <row r="26" spans="1:54" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="92" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" s="92"/>
+      <c r="C26" s="92"/>
+      <c r="D26" s="92"/>
+      <c r="E26" s="92"/>
+      <c r="F26" s="92"/>
+      <c r="G26" s="92"/>
+      <c r="H26" s="92"/>
+      <c r="I26" s="92"/>
+      <c r="J26" s="92"/>
+      <c r="K26" s="92"/>
+      <c r="L26" s="92"/>
+      <c r="M26" s="92"/>
+      <c r="N26" s="92"/>
+      <c r="O26" s="92"/>
+      <c r="P26" s="92"/>
+      <c r="Q26" s="92"/>
+      <c r="R26" s="92"/>
+      <c r="S26" s="92"/>
+      <c r="T26" s="92"/>
+      <c r="U26" s="92"/>
+      <c r="AC26" s="4"/>
+      <c r="AD26" s="4"/>
       <c r="AE26" s="4"/>
       <c r="AF26" s="4"/>
       <c r="AG26" s="4"/>
-      <c r="AH26" s="4"/>
-      <c r="AI26" s="4"/>
-      <c r="AJ26" s="56"/>
-      <c r="AK26" s="54"/>
+      <c r="AH26" s="50"/>
+      <c r="AI26" s="48"/>
+      <c r="AJ26" s="4"/>
+      <c r="AK26" s="49"/>
       <c r="AL26" s="4"/>
-      <c r="AM26" s="55"/>
+      <c r="AM26" s="49"/>
       <c r="AN26" s="4"/>
-      <c r="AO26" s="55"/>
+      <c r="AO26" s="49"/>
       <c r="AP26" s="4"/>
-      <c r="AQ26" s="55"/>
-      <c r="AR26" s="4"/>
-      <c r="AS26" s="55"/>
-      <c r="AT26" s="55"/>
-      <c r="AU26" s="56"/>
-      <c r="AV26" s="54"/>
+      <c r="AQ26" s="49"/>
+      <c r="AR26" s="49"/>
+      <c r="AS26" s="50"/>
+      <c r="AT26" s="48"/>
+      <c r="AU26" s="4"/>
+      <c r="AV26" s="49"/>
       <c r="AW26" s="4"/>
-      <c r="AX26" s="55"/>
+      <c r="AX26" s="49"/>
       <c r="AY26" s="4"/>
-      <c r="AZ26" s="55"/>
+      <c r="AZ26" s="49"/>
       <c r="BA26" s="4"/>
-      <c r="BB26" s="55"/>
-      <c r="BC26" s="4"/>
-      <c r="BD26" s="4"/>
-    </row>
-    <row r="27" spans="1:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="58"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
-      <c r="I27" s="15"/>
-      <c r="J27" s="15"/>
-      <c r="K27" s="15"/>
-      <c r="L27" s="59"/>
-      <c r="M27" s="15"/>
-      <c r="N27" s="16"/>
-      <c r="O27" s="60"/>
-      <c r="P27" s="60"/>
-      <c r="Q27" s="60"/>
-      <c r="R27" s="60"/>
-      <c r="S27" s="60"/>
-      <c r="T27" s="60"/>
-      <c r="U27" s="61"/>
+      <c r="BB26" s="4"/>
+    </row>
+    <row r="27" spans="1:54" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="74"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="75"/>
+      <c r="M27" s="7"/>
+      <c r="N27" s="7"/>
+      <c r="O27" s="55"/>
+      <c r="P27" s="55"/>
+      <c r="Q27" s="55"/>
+      <c r="R27" s="55"/>
+      <c r="S27" s="55"/>
+      <c r="T27" s="55"/>
+      <c r="U27" s="55"/>
+      <c r="V27" s="85" t="s">
+        <v>101</v>
+      </c>
+      <c r="W27" s="85" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC27" s="4"/>
+      <c r="AD27" s="4"/>
       <c r="AE27" s="4"/>
       <c r="AF27" s="4"/>
       <c r="AG27" s="4"/>
       <c r="AH27" s="4"/>
-      <c r="AI27" s="4"/>
-      <c r="AJ27" s="4"/>
-      <c r="AK27" s="54"/>
-      <c r="AL27" s="54"/>
-      <c r="AM27" s="55"/>
-      <c r="AN27" s="55"/>
-      <c r="AO27" s="55"/>
-      <c r="AP27" s="55"/>
-      <c r="AQ27" s="55"/>
-      <c r="AR27" s="55"/>
+      <c r="AI27" s="48"/>
+      <c r="AJ27" s="48"/>
+      <c r="AK27" s="49"/>
+      <c r="AL27" s="49"/>
+      <c r="AM27" s="49"/>
+      <c r="AN27" s="49"/>
+      <c r="AO27" s="49"/>
+      <c r="AP27" s="49"/>
+      <c r="AQ27" s="4"/>
+      <c r="AR27" s="4"/>
       <c r="AS27" s="4"/>
-      <c r="AT27" s="4"/>
-      <c r="AU27" s="4"/>
-      <c r="AV27" s="54"/>
-      <c r="AW27" s="54"/>
-      <c r="AX27" s="55"/>
-      <c r="AY27" s="55"/>
-      <c r="AZ27" s="55"/>
-      <c r="BA27" s="55"/>
-      <c r="BB27" s="55"/>
-      <c r="BC27" s="55"/>
-      <c r="BD27" s="4"/>
-    </row>
-    <row r="28" spans="1:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="69" t="s">
-        <v>82</v>
-      </c>
-      <c r="B28" s="70"/>
-      <c r="C28" s="70"/>
-      <c r="D28" s="70"/>
-      <c r="E28" s="70"/>
-      <c r="F28" s="70"/>
-      <c r="G28" s="70"/>
-      <c r="H28" s="70"/>
-      <c r="I28" s="70"/>
-      <c r="J28" s="70"/>
-      <c r="K28" s="70"/>
-      <c r="L28" s="71"/>
-      <c r="O28" s="60"/>
-      <c r="P28" s="60"/>
-      <c r="Q28" s="60"/>
-      <c r="R28" s="60"/>
-      <c r="S28" s="60"/>
-      <c r="T28" s="60"/>
-      <c r="U28" s="61"/>
+      <c r="AT27" s="48"/>
+      <c r="AU27" s="48"/>
+      <c r="AV27" s="49"/>
+      <c r="AW27" s="49"/>
+      <c r="AX27" s="49"/>
+      <c r="AY27" s="49"/>
+      <c r="AZ27" s="49"/>
+      <c r="BA27" s="49"/>
+      <c r="BB27" s="4"/>
+    </row>
+    <row r="28" spans="1:54" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="93" t="s">
+        <v>91</v>
+      </c>
+      <c r="B28" s="94"/>
+      <c r="C28" s="94"/>
+      <c r="D28" s="94"/>
+      <c r="E28" s="94"/>
+      <c r="F28" s="94"/>
+      <c r="G28" s="94"/>
+      <c r="H28" s="94"/>
+      <c r="I28" s="94"/>
+      <c r="J28" s="94"/>
+      <c r="K28" s="94"/>
+      <c r="L28" s="95"/>
+      <c r="M28" s="72" t="s">
+        <v>94</v>
+      </c>
+      <c r="N28" s="72"/>
+      <c r="O28" s="73"/>
+      <c r="P28" s="73"/>
+      <c r="Q28" s="73"/>
+      <c r="R28" s="73"/>
+      <c r="S28" s="73"/>
+      <c r="T28" s="73"/>
+      <c r="U28" s="73"/>
+      <c r="V28" s="21"/>
+      <c r="W28" s="21"/>
+      <c r="AC28" s="4"/>
+      <c r="AD28" s="4"/>
       <c r="AE28" s="4"/>
       <c r="AF28" s="4"/>
       <c r="AG28" s="4"/>
@@ -3321,38 +3450,40 @@
       <c r="AZ28" s="4"/>
       <c r="BA28" s="4"/>
       <c r="BB28" s="4"/>
-      <c r="BC28" s="4"/>
-      <c r="BD28" s="4"/>
-    </row>
-    <row r="29" spans="1:56" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A29" s="9"/>
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
-      <c r="G29" s="62" t="s">
-        <v>83</v>
+      <c r="G29" s="52" t="s">
+        <v>92</v>
       </c>
       <c r="I29" s="10"/>
       <c r="J29" s="10"/>
       <c r="K29" s="10"/>
       <c r="L29" s="10"/>
-      <c r="M29" s="72" t="s">
-        <v>84</v>
-      </c>
-      <c r="N29" s="73"/>
-      <c r="O29" s="74"/>
-      <c r="P29" s="75" t="s">
-        <v>85</v>
-      </c>
-      <c r="Q29" s="76"/>
-      <c r="R29" s="77"/>
-      <c r="S29" s="72" t="s">
-        <v>86</v>
-      </c>
-      <c r="T29" s="73"/>
-      <c r="U29" s="74"/>
+      <c r="M29" s="77" t="s">
+        <v>97</v>
+      </c>
+      <c r="N29" s="78"/>
+      <c r="O29" s="78"/>
+      <c r="P29" s="78"/>
+      <c r="Q29" s="78"/>
+      <c r="R29" s="78"/>
+      <c r="S29" s="78"/>
+      <c r="T29" s="78"/>
+      <c r="U29" s="78"/>
+      <c r="V29" s="85" t="s">
+        <v>103</v>
+      </c>
+      <c r="W29" s="85" t="s">
+        <v>104</v>
+      </c>
+      <c r="AC29" s="4"/>
+      <c r="AD29" s="4"/>
       <c r="AE29" s="4"/>
       <c r="AF29" s="4"/>
       <c r="AG29" s="4"/>
@@ -3377,401 +3508,447 @@
       <c r="AZ29" s="4"/>
       <c r="BA29" s="4"/>
       <c r="BB29" s="4"/>
-      <c r="BC29" s="4"/>
-      <c r="BD29" s="4"/>
-    </row>
-    <row r="30" spans="1:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="53"/>
+    </row>
+    <row r="30" spans="1:54" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="47"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
-      <c r="G30" s="63" t="s">
-        <v>87</v>
+      <c r="G30" s="53" t="s">
+        <v>74</v>
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
-      <c r="M30" s="53"/>
-      <c r="N30" s="1"/>
-      <c r="O30" s="64"/>
-      <c r="P30" s="53"/>
-      <c r="Q30" s="1"/>
-      <c r="R30" s="64"/>
-      <c r="S30" s="53"/>
-      <c r="T30" s="1"/>
-      <c r="U30" s="64"/>
+      <c r="M30" s="79" t="s">
+        <v>98</v>
+      </c>
+      <c r="N30" s="80"/>
+      <c r="O30" s="80"/>
+      <c r="P30" s="80"/>
+      <c r="Q30" s="80"/>
+      <c r="R30" s="80"/>
+      <c r="S30" s="80"/>
+      <c r="T30" s="80"/>
+      <c r="U30" s="80"/>
+      <c r="V30" s="21"/>
+      <c r="W30" s="21"/>
+      <c r="AC30" s="4"/>
+      <c r="AD30" s="4"/>
       <c r="AE30" s="4"/>
       <c r="AF30" s="4"/>
       <c r="AG30" s="4"/>
       <c r="AH30" s="4"/>
-      <c r="AI30" s="4"/>
-      <c r="AJ30" s="4"/>
-      <c r="AK30" s="54"/>
-      <c r="AL30" s="54"/>
-      <c r="AM30" s="55"/>
-      <c r="AN30" s="55"/>
-      <c r="AO30" s="55"/>
-      <c r="AP30" s="55"/>
-      <c r="AQ30" s="55"/>
-      <c r="AR30" s="55"/>
+      <c r="AI30" s="48"/>
+      <c r="AJ30" s="48"/>
+      <c r="AK30" s="49"/>
+      <c r="AL30" s="49"/>
+      <c r="AM30" s="49"/>
+      <c r="AN30" s="49"/>
+      <c r="AO30" s="49"/>
+      <c r="AP30" s="49"/>
+      <c r="AQ30" s="4"/>
+      <c r="AR30" s="4"/>
       <c r="AS30" s="4"/>
-      <c r="AT30" s="4"/>
-      <c r="AU30" s="4"/>
-      <c r="AV30" s="54"/>
-      <c r="AW30" s="54"/>
-      <c r="AX30" s="55"/>
-      <c r="AY30" s="55"/>
-      <c r="AZ30" s="55"/>
-      <c r="BA30" s="55"/>
-      <c r="BB30" s="55"/>
-      <c r="BC30" s="55"/>
-      <c r="BD30" s="4"/>
-    </row>
-    <row r="31" spans="1:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="53"/>
+      <c r="AT30" s="48"/>
+      <c r="AU30" s="48"/>
+      <c r="AV30" s="49"/>
+      <c r="AW30" s="49"/>
+      <c r="AX30" s="49"/>
+      <c r="AY30" s="49"/>
+      <c r="AZ30" s="49"/>
+      <c r="BA30" s="49"/>
+      <c r="BB30" s="4"/>
+    </row>
+    <row r="31" spans="1:54" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="47"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
-      <c r="G31" s="63" t="s">
-        <v>88</v>
+      <c r="G31" s="53" t="s">
+        <v>75</v>
       </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
-      <c r="M31" s="53"/>
-      <c r="N31" s="1"/>
-      <c r="O31" s="64"/>
-      <c r="P31" s="53"/>
-      <c r="Q31" s="1"/>
-      <c r="R31" s="64"/>
-      <c r="S31" s="53"/>
-      <c r="T31" s="1"/>
-      <c r="U31" s="64"/>
+      <c r="M31" s="76" t="s">
+        <v>99</v>
+      </c>
+      <c r="N31" s="10"/>
+      <c r="O31" s="10"/>
+      <c r="P31" s="10"/>
+      <c r="Q31" s="10"/>
+      <c r="R31" s="10"/>
+      <c r="S31" s="10"/>
+      <c r="T31" s="10"/>
+      <c r="U31" s="10"/>
+      <c r="V31" s="21"/>
+      <c r="W31" s="21"/>
+      <c r="AC31" s="4"/>
+      <c r="AD31" s="4"/>
       <c r="AE31" s="4"/>
       <c r="AF31" s="4"/>
       <c r="AG31" s="4"/>
-      <c r="AH31" s="4"/>
-      <c r="AI31" s="4"/>
-      <c r="AJ31" s="56"/>
-      <c r="AK31" s="54"/>
-      <c r="AL31" s="54"/>
-      <c r="AM31" s="55"/>
-      <c r="AN31" s="55"/>
-      <c r="AO31" s="55"/>
-      <c r="AP31" s="55"/>
-      <c r="AQ31" s="55"/>
-      <c r="AR31" s="55"/>
-      <c r="AS31" s="4"/>
-      <c r="AT31" s="4"/>
-      <c r="AU31" s="56"/>
-      <c r="AV31" s="54"/>
-      <c r="AW31" s="54"/>
-      <c r="AX31" s="55"/>
-      <c r="AY31" s="55"/>
-      <c r="AZ31" s="55"/>
-      <c r="BA31" s="55"/>
-      <c r="BB31" s="55"/>
-      <c r="BC31" s="55"/>
-      <c r="BD31" s="4"/>
-    </row>
-    <row r="32" spans="1:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="53"/>
+      <c r="AH31" s="50"/>
+      <c r="AI31" s="48"/>
+      <c r="AJ31" s="48"/>
+      <c r="AK31" s="49"/>
+      <c r="AL31" s="49"/>
+      <c r="AM31" s="49"/>
+      <c r="AN31" s="49"/>
+      <c r="AO31" s="49"/>
+      <c r="AP31" s="49"/>
+      <c r="AQ31" s="4"/>
+      <c r="AR31" s="4"/>
+      <c r="AS31" s="50"/>
+      <c r="AT31" s="48"/>
+      <c r="AU31" s="48"/>
+      <c r="AV31" s="49"/>
+      <c r="AW31" s="49"/>
+      <c r="AX31" s="49"/>
+      <c r="AY31" s="49"/>
+      <c r="AZ31" s="49"/>
+      <c r="BA31" s="49"/>
+      <c r="BB31" s="4"/>
+    </row>
+    <row r="32" spans="1:54" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="47"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
-      <c r="G32" s="63" t="s">
-        <v>89</v>
+      <c r="G32" s="53" t="s">
+        <v>76</v>
       </c>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
-      <c r="M32" s="53"/>
-      <c r="N32" s="1"/>
-      <c r="O32" s="64"/>
-      <c r="P32" s="53"/>
-      <c r="Q32" s="1"/>
-      <c r="R32" s="64"/>
-      <c r="S32" s="53"/>
-      <c r="T32" s="1"/>
-      <c r="U32" s="64"/>
+      <c r="M32" s="84" t="s">
+        <v>100</v>
+      </c>
+      <c r="N32" s="81"/>
+      <c r="O32" s="81"/>
+      <c r="P32" s="82"/>
+      <c r="Q32" s="82"/>
+      <c r="R32" s="82"/>
+      <c r="S32" s="83"/>
+      <c r="T32" s="83"/>
+      <c r="U32" s="83"/>
+      <c r="V32" s="85" t="s">
+        <v>103</v>
+      </c>
+      <c r="W32" s="85" t="s">
+        <v>104</v>
+      </c>
+      <c r="AC32" s="4"/>
+      <c r="AD32" s="4"/>
       <c r="AE32" s="4"/>
       <c r="AF32" s="4"/>
       <c r="AG32" s="4"/>
-      <c r="AH32" s="4"/>
-      <c r="AI32" s="4"/>
-      <c r="AJ32" s="54"/>
-      <c r="AK32" s="54"/>
-      <c r="AL32" s="54"/>
-      <c r="AM32" s="55"/>
-      <c r="AN32" s="55"/>
-      <c r="AO32" s="55"/>
-      <c r="AP32" s="55"/>
-      <c r="AQ32" s="55"/>
-      <c r="AR32" s="55"/>
-      <c r="AS32" s="4"/>
-      <c r="AT32" s="4"/>
-      <c r="AU32" s="54"/>
-      <c r="AV32" s="54"/>
-      <c r="AW32" s="54"/>
-      <c r="AX32" s="55"/>
-      <c r="AY32" s="55"/>
-      <c r="AZ32" s="55"/>
-      <c r="BA32" s="55"/>
-      <c r="BB32" s="55"/>
-      <c r="BC32" s="55"/>
-      <c r="BD32" s="4"/>
-    </row>
-    <row r="33" spans="1:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="57"/>
+      <c r="AH32" s="48"/>
+      <c r="AI32" s="48"/>
+      <c r="AJ32" s="48"/>
+      <c r="AK32" s="49"/>
+      <c r="AL32" s="49"/>
+      <c r="AM32" s="49"/>
+      <c r="AN32" s="49"/>
+      <c r="AO32" s="49"/>
+      <c r="AP32" s="49"/>
+      <c r="AQ32" s="4"/>
+      <c r="AR32" s="4"/>
+      <c r="AS32" s="48"/>
+      <c r="AT32" s="48"/>
+      <c r="AU32" s="48"/>
+      <c r="AV32" s="49"/>
+      <c r="AW32" s="49"/>
+      <c r="AX32" s="49"/>
+      <c r="AY32" s="49"/>
+      <c r="AZ32" s="49"/>
+      <c r="BA32" s="49"/>
+      <c r="BB32" s="4"/>
+    </row>
+    <row r="33" spans="1:54" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="51"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
-      <c r="G33" s="65" t="s">
-        <v>90</v>
+      <c r="G33" s="54" t="s">
+        <v>93</v>
       </c>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
       <c r="J33" s="7"/>
       <c r="K33" s="7"/>
       <c r="L33" s="7"/>
-      <c r="M33" s="57"/>
-      <c r="N33" s="7"/>
-      <c r="O33" s="8"/>
-      <c r="P33" s="57"/>
-      <c r="Q33" s="7"/>
-      <c r="R33" s="8"/>
-      <c r="S33" s="57"/>
-      <c r="T33" s="7"/>
-      <c r="U33" s="8"/>
+      <c r="M33" s="86" t="s">
+        <v>73</v>
+      </c>
+      <c r="N33" s="87"/>
+      <c r="O33" s="88"/>
+      <c r="P33" s="89" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q33" s="90"/>
+      <c r="R33" s="91"/>
+      <c r="S33" s="86" t="s">
+        <v>96</v>
+      </c>
+      <c r="T33" s="87"/>
+      <c r="U33" s="87"/>
+      <c r="V33" s="85"/>
+      <c r="W33" s="21"/>
+      <c r="AC33" s="4"/>
+      <c r="AD33" s="4"/>
       <c r="AE33" s="4"/>
       <c r="AF33" s="4"/>
       <c r="AG33" s="4"/>
       <c r="AH33" s="4"/>
-      <c r="AI33" s="4"/>
-      <c r="AJ33" s="4"/>
-      <c r="AK33" s="54"/>
-      <c r="AL33" s="54"/>
-      <c r="AM33" s="55"/>
-      <c r="AN33" s="55"/>
-      <c r="AO33" s="55"/>
-      <c r="AP33" s="55"/>
-      <c r="AQ33" s="55"/>
-      <c r="AR33" s="55"/>
+      <c r="AI33" s="48"/>
+      <c r="AJ33" s="48"/>
+      <c r="AK33" s="49"/>
+      <c r="AL33" s="49"/>
+      <c r="AM33" s="49"/>
+      <c r="AN33" s="49"/>
+      <c r="AO33" s="49"/>
+      <c r="AP33" s="49"/>
+      <c r="AQ33" s="4"/>
+      <c r="AR33" s="4"/>
       <c r="AS33" s="4"/>
-      <c r="AT33" s="4"/>
-      <c r="AU33" s="4"/>
-      <c r="AV33" s="54"/>
-      <c r="AW33" s="54"/>
-      <c r="AX33" s="55"/>
-      <c r="AY33" s="55"/>
-      <c r="AZ33" s="55"/>
-      <c r="BA33" s="55"/>
-      <c r="BB33" s="55"/>
-      <c r="BC33" s="55"/>
-      <c r="BD33" s="4"/>
-    </row>
-    <row r="34" spans="1:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AT33" s="48"/>
+      <c r="AU33" s="48"/>
+      <c r="AV33" s="49"/>
+      <c r="AW33" s="49"/>
+      <c r="AX33" s="49"/>
+      <c r="AY33" s="49"/>
+      <c r="AZ33" s="49"/>
+      <c r="BA33" s="49"/>
+      <c r="BB33" s="4"/>
+    </row>
+    <row r="34" spans="1:54" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M34" s="68"/>
+      <c r="N34" s="69"/>
+      <c r="O34" s="70"/>
+      <c r="P34" s="68"/>
+      <c r="Q34" s="69"/>
+      <c r="R34" s="70"/>
+      <c r="S34" s="68"/>
+      <c r="T34" s="69"/>
+      <c r="U34" s="69"/>
+      <c r="V34" s="21"/>
+      <c r="W34" s="21"/>
+      <c r="AC34" s="4"/>
+      <c r="AD34" s="4"/>
       <c r="AE34" s="4"/>
       <c r="AF34" s="4"/>
       <c r="AG34" s="4"/>
       <c r="AH34" s="4"/>
-      <c r="AI34" s="4"/>
-      <c r="AJ34" s="4"/>
-      <c r="AK34" s="54"/>
-      <c r="AL34" s="54"/>
-      <c r="AM34" s="55"/>
-      <c r="AN34" s="55"/>
-      <c r="AO34" s="55"/>
-      <c r="AP34" s="55"/>
-      <c r="AQ34" s="55"/>
-      <c r="AR34" s="55"/>
+      <c r="AI34" s="48"/>
+      <c r="AJ34" s="48"/>
+      <c r="AK34" s="49"/>
+      <c r="AL34" s="49"/>
+      <c r="AM34" s="49"/>
+      <c r="AN34" s="49"/>
+      <c r="AO34" s="49"/>
+      <c r="AP34" s="49"/>
+      <c r="AQ34" s="4"/>
+      <c r="AR34" s="4"/>
       <c r="AS34" s="4"/>
-      <c r="AT34" s="4"/>
-      <c r="AU34" s="4"/>
-      <c r="AV34" s="54"/>
-      <c r="AW34" s="54"/>
-      <c r="AX34" s="55"/>
-      <c r="AY34" s="55"/>
-      <c r="AZ34" s="55"/>
-      <c r="BA34" s="55"/>
-      <c r="BB34" s="55"/>
-      <c r="BC34" s="55"/>
-      <c r="BD34" s="4"/>
-    </row>
-    <row r="35" spans="1:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AT34" s="48"/>
+      <c r="AU34" s="48"/>
+      <c r="AV34" s="49"/>
+      <c r="AW34" s="49"/>
+      <c r="AX34" s="49"/>
+      <c r="AY34" s="49"/>
+      <c r="AZ34" s="49"/>
+      <c r="BA34" s="49"/>
+      <c r="BB34" s="4"/>
+    </row>
+    <row r="35" spans="1:54" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M35" s="68"/>
+      <c r="N35" s="69"/>
+      <c r="O35" s="70"/>
+      <c r="P35" s="71"/>
+      <c r="Q35" s="71"/>
+      <c r="R35" s="70"/>
+      <c r="S35" s="71"/>
+      <c r="T35" s="71"/>
+      <c r="U35" s="71"/>
+      <c r="V35" s="21"/>
+      <c r="W35" s="21"/>
+      <c r="AC35" s="4"/>
+      <c r="AD35" s="4"/>
       <c r="AE35" s="4"/>
       <c r="AF35" s="4"/>
       <c r="AG35" s="4"/>
-      <c r="AH35" s="4"/>
-      <c r="AI35" s="4"/>
-      <c r="AJ35" s="56"/>
-      <c r="AK35" s="54"/>
-      <c r="AL35" s="54"/>
-      <c r="AM35" s="55"/>
-      <c r="AN35" s="55"/>
-      <c r="AO35" s="55"/>
-      <c r="AP35" s="55"/>
-      <c r="AQ35" s="55"/>
-      <c r="AR35" s="55"/>
-      <c r="AS35" s="4"/>
-      <c r="AT35" s="4"/>
-      <c r="AU35" s="56"/>
-      <c r="AV35" s="54"/>
-      <c r="AW35" s="54"/>
-      <c r="AX35" s="55"/>
-      <c r="AY35" s="55"/>
-      <c r="AZ35" s="55"/>
-      <c r="BA35" s="55"/>
-      <c r="BB35" s="55"/>
-      <c r="BC35" s="55"/>
-      <c r="BD35" s="4"/>
-    </row>
-    <row r="36" spans="1:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH35" s="50"/>
+      <c r="AI35" s="48"/>
+      <c r="AJ35" s="48"/>
+      <c r="AK35" s="49"/>
+      <c r="AL35" s="49"/>
+      <c r="AM35" s="49"/>
+      <c r="AN35" s="49"/>
+      <c r="AO35" s="49"/>
+      <c r="AP35" s="49"/>
+      <c r="AQ35" s="4"/>
+      <c r="AR35" s="4"/>
+      <c r="AS35" s="50"/>
+      <c r="AT35" s="48"/>
+      <c r="AU35" s="48"/>
+      <c r="AV35" s="49"/>
+      <c r="AW35" s="49"/>
+      <c r="AX35" s="49"/>
+      <c r="AY35" s="49"/>
+      <c r="AZ35" s="49"/>
+      <c r="BA35" s="49"/>
+      <c r="BB35" s="4"/>
+    </row>
+    <row r="36" spans="1:54" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC36" s="4"/>
+      <c r="AD36" s="4"/>
       <c r="AE36" s="4"/>
       <c r="AF36" s="4"/>
       <c r="AG36" s="4"/>
       <c r="AH36" s="4"/>
-      <c r="AI36" s="4"/>
-      <c r="AJ36" s="4"/>
-      <c r="AK36" s="54"/>
-      <c r="AL36" s="54"/>
-      <c r="AM36" s="55"/>
-      <c r="AN36" s="55"/>
-      <c r="AO36" s="55"/>
-      <c r="AP36" s="55"/>
-      <c r="AQ36" s="55"/>
-      <c r="AR36" s="55"/>
+      <c r="AI36" s="48"/>
+      <c r="AJ36" s="48"/>
+      <c r="AK36" s="49"/>
+      <c r="AL36" s="49"/>
+      <c r="AM36" s="49"/>
+      <c r="AN36" s="49"/>
+      <c r="AO36" s="49"/>
+      <c r="AP36" s="49"/>
+      <c r="AQ36" s="4"/>
+      <c r="AR36" s="4"/>
       <c r="AS36" s="4"/>
-      <c r="AT36" s="4"/>
-      <c r="AU36" s="4"/>
-      <c r="AV36" s="54"/>
-      <c r="AW36" s="54"/>
-      <c r="AX36" s="55"/>
-      <c r="AY36" s="55"/>
-      <c r="AZ36" s="55"/>
-      <c r="BA36" s="55"/>
-      <c r="BB36" s="55"/>
-      <c r="BC36" s="55"/>
-      <c r="BD36" s="4"/>
-    </row>
-    <row r="37" spans="1:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AT36" s="48"/>
+      <c r="AU36" s="48"/>
+      <c r="AV36" s="49"/>
+      <c r="AW36" s="49"/>
+      <c r="AX36" s="49"/>
+      <c r="AY36" s="49"/>
+      <c r="AZ36" s="49"/>
+      <c r="BA36" s="49"/>
+      <c r="BB36" s="4"/>
+    </row>
+    <row r="37" spans="1:54" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC37" s="4"/>
+      <c r="AD37" s="4"/>
       <c r="AE37" s="4"/>
       <c r="AF37" s="4"/>
       <c r="AG37" s="4"/>
       <c r="AH37" s="4"/>
-      <c r="AI37" s="4"/>
-      <c r="AJ37" s="4"/>
-      <c r="AK37" s="54"/>
-      <c r="AL37" s="54"/>
-      <c r="AM37" s="55"/>
-      <c r="AN37" s="55"/>
-      <c r="AO37" s="55"/>
-      <c r="AP37" s="55"/>
-      <c r="AQ37" s="55"/>
-      <c r="AR37" s="55"/>
+      <c r="AI37" s="48"/>
+      <c r="AJ37" s="48"/>
+      <c r="AK37" s="49"/>
+      <c r="AL37" s="49"/>
+      <c r="AM37" s="49"/>
+      <c r="AN37" s="49"/>
+      <c r="AO37" s="49"/>
+      <c r="AP37" s="49"/>
+      <c r="AQ37" s="4"/>
+      <c r="AR37" s="4"/>
       <c r="AS37" s="4"/>
-      <c r="AT37" s="4"/>
-      <c r="AU37" s="4"/>
-      <c r="AV37" s="54"/>
-      <c r="AW37" s="54"/>
-      <c r="AX37" s="55"/>
-      <c r="AY37" s="55"/>
-      <c r="AZ37" s="55"/>
-      <c r="BA37" s="55"/>
-      <c r="BB37" s="55"/>
-      <c r="BC37" s="55"/>
-      <c r="BD37" s="4"/>
-    </row>
-    <row r="38" spans="1:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AT37" s="48"/>
+      <c r="AU37" s="48"/>
+      <c r="AV37" s="49"/>
+      <c r="AW37" s="49"/>
+      <c r="AX37" s="49"/>
+      <c r="AY37" s="49"/>
+      <c r="AZ37" s="49"/>
+      <c r="BA37" s="49"/>
+      <c r="BB37" s="4"/>
+    </row>
+    <row r="38" spans="1:54" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC38" s="4"/>
+      <c r="AD38" s="4"/>
       <c r="AE38" s="4"/>
       <c r="AF38" s="4"/>
       <c r="AG38" s="4"/>
-      <c r="AH38" s="4"/>
-      <c r="AI38" s="4"/>
-      <c r="AJ38" s="54"/>
-      <c r="AK38" s="54"/>
-      <c r="AL38" s="54"/>
-      <c r="AM38" s="55"/>
-      <c r="AN38" s="55"/>
-      <c r="AO38" s="55"/>
-      <c r="AP38" s="55"/>
-      <c r="AQ38" s="55"/>
-      <c r="AR38" s="55"/>
-      <c r="AS38" s="4"/>
-      <c r="AT38" s="4"/>
-      <c r="AU38" s="54"/>
-      <c r="AV38" s="54"/>
-      <c r="AW38" s="54"/>
-      <c r="AX38" s="55"/>
-      <c r="AY38" s="55"/>
-      <c r="AZ38" s="55"/>
-      <c r="BA38" s="55"/>
-      <c r="BB38" s="55"/>
-      <c r="BC38" s="55"/>
-      <c r="BD38" s="4"/>
-    </row>
-    <row r="39" spans="1:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH38" s="48"/>
+      <c r="AI38" s="48"/>
+      <c r="AJ38" s="48"/>
+      <c r="AK38" s="49"/>
+      <c r="AL38" s="49"/>
+      <c r="AM38" s="49"/>
+      <c r="AN38" s="49"/>
+      <c r="AO38" s="49"/>
+      <c r="AP38" s="49"/>
+      <c r="AQ38" s="4"/>
+      <c r="AR38" s="4"/>
+      <c r="AS38" s="48"/>
+      <c r="AT38" s="48"/>
+      <c r="AU38" s="48"/>
+      <c r="AV38" s="49"/>
+      <c r="AW38" s="49"/>
+      <c r="AX38" s="49"/>
+      <c r="AY38" s="49"/>
+      <c r="AZ38" s="49"/>
+      <c r="BA38" s="49"/>
+      <c r="BB38" s="4"/>
+    </row>
+    <row r="39" spans="1:54" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC39" s="4"/>
+      <c r="AD39" s="4"/>
       <c r="AE39" s="4"/>
       <c r="AF39" s="4"/>
       <c r="AG39" s="4"/>
-      <c r="AH39" s="4"/>
-      <c r="AI39" s="4"/>
-      <c r="AJ39" s="56"/>
-      <c r="AK39" s="54"/>
+      <c r="AH39" s="50"/>
+      <c r="AI39" s="48"/>
+      <c r="AJ39" s="4"/>
+      <c r="AK39" s="49"/>
       <c r="AL39" s="4"/>
-      <c r="AM39" s="55"/>
+      <c r="AM39" s="49"/>
       <c r="AN39" s="4"/>
-      <c r="AO39" s="55"/>
+      <c r="AO39" s="49"/>
       <c r="AP39" s="4"/>
-      <c r="AQ39" s="55"/>
+      <c r="AQ39" s="4"/>
       <c r="AR39" s="4"/>
-      <c r="AS39" s="4"/>
-      <c r="AT39" s="4"/>
-      <c r="AU39" s="56"/>
-      <c r="AV39" s="54"/>
+      <c r="AS39" s="50"/>
+      <c r="AT39" s="48"/>
+      <c r="AU39" s="4"/>
+      <c r="AV39" s="49"/>
       <c r="AW39" s="4"/>
-      <c r="AX39" s="55"/>
+      <c r="AX39" s="49"/>
       <c r="AY39" s="4"/>
-      <c r="AZ39" s="55"/>
+      <c r="AZ39" s="49"/>
       <c r="BA39" s="4"/>
-      <c r="BB39" s="55"/>
-      <c r="BC39" s="4"/>
-      <c r="BD39" s="4"/>
-    </row>
-    <row r="40" spans="1:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BB39" s="4"/>
+    </row>
+    <row r="40" spans="1:54" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC40" s="4"/>
+      <c r="AD40" s="4"/>
       <c r="AE40" s="4"/>
       <c r="AF40" s="4"/>
       <c r="AG40" s="4"/>
       <c r="AH40" s="4"/>
-      <c r="AI40" s="4"/>
-      <c r="AJ40" s="4"/>
-      <c r="AK40" s="54"/>
-      <c r="AL40" s="54"/>
-      <c r="AM40" s="55"/>
-      <c r="AN40" s="55"/>
-      <c r="AO40" s="55"/>
-      <c r="AP40" s="55"/>
-      <c r="AQ40" s="55"/>
-      <c r="AR40" s="55"/>
+      <c r="AI40" s="48"/>
+      <c r="AJ40" s="48"/>
+      <c r="AK40" s="49"/>
+      <c r="AL40" s="49"/>
+      <c r="AM40" s="49"/>
+      <c r="AN40" s="49"/>
+      <c r="AO40" s="49"/>
+      <c r="AP40" s="49"/>
+      <c r="AQ40" s="4"/>
+      <c r="AR40" s="4"/>
       <c r="AS40" s="4"/>
-      <c r="AT40" s="4"/>
-      <c r="AU40" s="4"/>
-      <c r="AV40" s="54"/>
-      <c r="AW40" s="54"/>
-      <c r="AX40" s="55"/>
-      <c r="AY40" s="55"/>
-      <c r="AZ40" s="55"/>
-      <c r="BA40" s="55"/>
-      <c r="BB40" s="55"/>
-      <c r="BC40" s="55"/>
-      <c r="BD40" s="4"/>
-    </row>
-    <row r="41" spans="1:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AT40" s="48"/>
+      <c r="AU40" s="48"/>
+      <c r="AV40" s="49"/>
+      <c r="AW40" s="49"/>
+      <c r="AX40" s="49"/>
+      <c r="AY40" s="49"/>
+      <c r="AZ40" s="49"/>
+      <c r="BA40" s="49"/>
+      <c r="BB40" s="4"/>
+    </row>
+    <row r="41" spans="1:54" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC41" s="4"/>
+      <c r="AD41" s="4"/>
       <c r="AE41" s="4"/>
       <c r="AF41" s="4"/>
       <c r="AG41" s="4"/>
@@ -3796,10 +3973,10 @@
       <c r="AZ41" s="4"/>
       <c r="BA41" s="4"/>
       <c r="BB41" s="4"/>
-      <c r="BC41" s="4"/>
-      <c r="BD41" s="4"/>
-    </row>
-    <row r="42" spans="1:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:54" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC42" s="4"/>
+      <c r="AD42" s="4"/>
       <c r="AE42" s="4"/>
       <c r="AF42" s="4"/>
       <c r="AG42" s="4"/>
@@ -3824,318 +4001,318 @@
       <c r="AZ42" s="4"/>
       <c r="BA42" s="4"/>
       <c r="BB42" s="4"/>
-      <c r="BC42" s="4"/>
-      <c r="BD42" s="4"/>
-    </row>
-    <row r="43" spans="1:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:54" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC43" s="4"/>
+      <c r="AD43" s="4"/>
       <c r="AE43" s="4"/>
       <c r="AF43" s="4"/>
       <c r="AG43" s="4"/>
       <c r="AH43" s="4"/>
-      <c r="AI43" s="4"/>
-      <c r="AJ43" s="4"/>
-      <c r="AK43" s="54"/>
-      <c r="AL43" s="54"/>
-      <c r="AM43" s="55"/>
-      <c r="AN43" s="55"/>
-      <c r="AO43" s="55"/>
-      <c r="AP43" s="55"/>
-      <c r="AQ43" s="55"/>
-      <c r="AR43" s="55"/>
+      <c r="AI43" s="48"/>
+      <c r="AJ43" s="48"/>
+      <c r="AK43" s="49"/>
+      <c r="AL43" s="49"/>
+      <c r="AM43" s="49"/>
+      <c r="AN43" s="49"/>
+      <c r="AO43" s="49"/>
+      <c r="AP43" s="49"/>
+      <c r="AQ43" s="4"/>
+      <c r="AR43" s="4"/>
       <c r="AS43" s="4"/>
-      <c r="AT43" s="4"/>
-      <c r="AU43" s="4"/>
-      <c r="AV43" s="54"/>
-      <c r="AW43" s="54"/>
-      <c r="AX43" s="55"/>
-      <c r="AY43" s="55"/>
-      <c r="AZ43" s="55"/>
-      <c r="BA43" s="55"/>
-      <c r="BB43" s="55"/>
-      <c r="BC43" s="55"/>
-      <c r="BD43" s="4"/>
-    </row>
-    <row r="44" spans="1:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AT43" s="48"/>
+      <c r="AU43" s="48"/>
+      <c r="AV43" s="49"/>
+      <c r="AW43" s="49"/>
+      <c r="AX43" s="49"/>
+      <c r="AY43" s="49"/>
+      <c r="AZ43" s="49"/>
+      <c r="BA43" s="49"/>
+      <c r="BB43" s="4"/>
+    </row>
+    <row r="44" spans="1:54" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC44" s="4"/>
+      <c r="AD44" s="4"/>
       <c r="AE44" s="4"/>
       <c r="AF44" s="4"/>
       <c r="AG44" s="4"/>
-      <c r="AH44" s="4"/>
-      <c r="AI44" s="4"/>
-      <c r="AJ44" s="56"/>
-      <c r="AK44" s="54"/>
-      <c r="AL44" s="54"/>
-      <c r="AM44" s="55"/>
-      <c r="AN44" s="55"/>
-      <c r="AO44" s="55"/>
-      <c r="AP44" s="55"/>
-      <c r="AQ44" s="55"/>
-      <c r="AR44" s="55"/>
-      <c r="AS44" s="4"/>
-      <c r="AT44" s="4"/>
-      <c r="AU44" s="56"/>
-      <c r="AV44" s="54"/>
-      <c r="AW44" s="54"/>
-      <c r="AX44" s="55"/>
-      <c r="AY44" s="55"/>
-      <c r="AZ44" s="55"/>
-      <c r="BA44" s="55"/>
-      <c r="BB44" s="55"/>
-      <c r="BC44" s="55"/>
-      <c r="BD44" s="4"/>
-    </row>
-    <row r="45" spans="1:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH44" s="50"/>
+      <c r="AI44" s="48"/>
+      <c r="AJ44" s="48"/>
+      <c r="AK44" s="49"/>
+      <c r="AL44" s="49"/>
+      <c r="AM44" s="49"/>
+      <c r="AN44" s="49"/>
+      <c r="AO44" s="49"/>
+      <c r="AP44" s="49"/>
+      <c r="AQ44" s="4"/>
+      <c r="AR44" s="4"/>
+      <c r="AS44" s="50"/>
+      <c r="AT44" s="48"/>
+      <c r="AU44" s="48"/>
+      <c r="AV44" s="49"/>
+      <c r="AW44" s="49"/>
+      <c r="AX44" s="49"/>
+      <c r="AY44" s="49"/>
+      <c r="AZ44" s="49"/>
+      <c r="BA44" s="49"/>
+      <c r="BB44" s="4"/>
+    </row>
+    <row r="45" spans="1:54" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC45" s="4"/>
+      <c r="AD45" s="4"/>
       <c r="AE45" s="4"/>
       <c r="AF45" s="4"/>
       <c r="AG45" s="4"/>
-      <c r="AH45" s="4"/>
-      <c r="AI45" s="4"/>
-      <c r="AJ45" s="54"/>
-      <c r="AK45" s="54"/>
-      <c r="AL45" s="54"/>
-      <c r="AM45" s="55"/>
-      <c r="AN45" s="55"/>
-      <c r="AO45" s="55"/>
-      <c r="AP45" s="55"/>
-      <c r="AQ45" s="55"/>
-      <c r="AR45" s="55"/>
-      <c r="AS45" s="4"/>
-      <c r="AT45" s="4"/>
-      <c r="AU45" s="54"/>
-      <c r="AV45" s="54"/>
-      <c r="AW45" s="54"/>
-      <c r="AX45" s="55"/>
-      <c r="AY45" s="55"/>
-      <c r="AZ45" s="55"/>
-      <c r="BA45" s="55"/>
-      <c r="BB45" s="55"/>
-      <c r="BC45" s="55"/>
-      <c r="BD45" s="4"/>
-    </row>
-    <row r="46" spans="1:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH45" s="48"/>
+      <c r="AI45" s="48"/>
+      <c r="AJ45" s="48"/>
+      <c r="AK45" s="49"/>
+      <c r="AL45" s="49"/>
+      <c r="AM45" s="49"/>
+      <c r="AN45" s="49"/>
+      <c r="AO45" s="49"/>
+      <c r="AP45" s="49"/>
+      <c r="AQ45" s="4"/>
+      <c r="AR45" s="4"/>
+      <c r="AS45" s="48"/>
+      <c r="AT45" s="48"/>
+      <c r="AU45" s="48"/>
+      <c r="AV45" s="49"/>
+      <c r="AW45" s="49"/>
+      <c r="AX45" s="49"/>
+      <c r="AY45" s="49"/>
+      <c r="AZ45" s="49"/>
+      <c r="BA45" s="49"/>
+      <c r="BB45" s="4"/>
+    </row>
+    <row r="46" spans="1:54" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC46" s="4"/>
+      <c r="AD46" s="4"/>
       <c r="AE46" s="4"/>
       <c r="AF46" s="4"/>
       <c r="AG46" s="4"/>
       <c r="AH46" s="4"/>
-      <c r="AI46" s="4"/>
-      <c r="AJ46" s="4"/>
-      <c r="AK46" s="54"/>
-      <c r="AL46" s="54"/>
-      <c r="AM46" s="55"/>
-      <c r="AN46" s="55"/>
-      <c r="AO46" s="55"/>
-      <c r="AP46" s="55"/>
-      <c r="AQ46" s="55"/>
-      <c r="AR46" s="55"/>
+      <c r="AI46" s="48"/>
+      <c r="AJ46" s="48"/>
+      <c r="AK46" s="49"/>
+      <c r="AL46" s="49"/>
+      <c r="AM46" s="49"/>
+      <c r="AN46" s="49"/>
+      <c r="AO46" s="49"/>
+      <c r="AP46" s="49"/>
+      <c r="AQ46" s="4"/>
+      <c r="AR46" s="4"/>
       <c r="AS46" s="4"/>
-      <c r="AT46" s="4"/>
-      <c r="AU46" s="4"/>
-      <c r="AV46" s="54"/>
-      <c r="AW46" s="54"/>
-      <c r="AX46" s="55"/>
-      <c r="AY46" s="55"/>
-      <c r="AZ46" s="55"/>
-      <c r="BA46" s="55"/>
-      <c r="BB46" s="55"/>
-      <c r="BC46" s="55"/>
-      <c r="BD46" s="4"/>
-    </row>
-    <row r="47" spans="1:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AT46" s="48"/>
+      <c r="AU46" s="48"/>
+      <c r="AV46" s="49"/>
+      <c r="AW46" s="49"/>
+      <c r="AX46" s="49"/>
+      <c r="AY46" s="49"/>
+      <c r="AZ46" s="49"/>
+      <c r="BA46" s="49"/>
+      <c r="BB46" s="4"/>
+    </row>
+    <row r="47" spans="1:54" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC47" s="4"/>
+      <c r="AD47" s="4"/>
       <c r="AE47" s="4"/>
       <c r="AF47" s="4"/>
       <c r="AG47" s="4"/>
       <c r="AH47" s="4"/>
-      <c r="AI47" s="4"/>
-      <c r="AJ47" s="4"/>
-      <c r="AK47" s="54"/>
-      <c r="AL47" s="54"/>
-      <c r="AM47" s="55"/>
-      <c r="AN47" s="55"/>
-      <c r="AO47" s="55"/>
-      <c r="AP47" s="55"/>
-      <c r="AQ47" s="55"/>
-      <c r="AR47" s="55"/>
+      <c r="AI47" s="48"/>
+      <c r="AJ47" s="48"/>
+      <c r="AK47" s="49"/>
+      <c r="AL47" s="49"/>
+      <c r="AM47" s="49"/>
+      <c r="AN47" s="49"/>
+      <c r="AO47" s="49"/>
+      <c r="AP47" s="49"/>
+      <c r="AQ47" s="4"/>
+      <c r="AR47" s="4"/>
       <c r="AS47" s="4"/>
-      <c r="AT47" s="4"/>
-      <c r="AU47" s="4"/>
-      <c r="AV47" s="54"/>
-      <c r="AW47" s="54"/>
-      <c r="AX47" s="55"/>
-      <c r="AY47" s="55"/>
-      <c r="AZ47" s="55"/>
-      <c r="BA47" s="55"/>
-      <c r="BB47" s="55"/>
-      <c r="BC47" s="55"/>
-      <c r="BD47" s="4"/>
-    </row>
-    <row r="48" spans="1:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AT47" s="48"/>
+      <c r="AU47" s="48"/>
+      <c r="AV47" s="49"/>
+      <c r="AW47" s="49"/>
+      <c r="AX47" s="49"/>
+      <c r="AY47" s="49"/>
+      <c r="AZ47" s="49"/>
+      <c r="BA47" s="49"/>
+      <c r="BB47" s="4"/>
+    </row>
+    <row r="48" spans="1:54" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC48" s="4"/>
+      <c r="AD48" s="4"/>
       <c r="AE48" s="4"/>
       <c r="AF48" s="4"/>
       <c r="AG48" s="4"/>
-      <c r="AH48" s="4"/>
-      <c r="AI48" s="4"/>
-      <c r="AJ48" s="56"/>
-      <c r="AK48" s="54"/>
-      <c r="AL48" s="54"/>
-      <c r="AM48" s="55"/>
-      <c r="AN48" s="55"/>
-      <c r="AO48" s="55"/>
-      <c r="AP48" s="55"/>
-      <c r="AQ48" s="55"/>
-      <c r="AR48" s="55"/>
-      <c r="AS48" s="4"/>
-      <c r="AT48" s="4"/>
-      <c r="AU48" s="56"/>
-      <c r="AV48" s="54"/>
-      <c r="AW48" s="54"/>
-      <c r="AX48" s="55"/>
-      <c r="AY48" s="55"/>
-      <c r="AZ48" s="55"/>
-      <c r="BA48" s="55"/>
-      <c r="BB48" s="55"/>
-      <c r="BC48" s="55"/>
-      <c r="BD48" s="4"/>
-    </row>
-    <row r="49" spans="31:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH48" s="50"/>
+      <c r="AI48" s="48"/>
+      <c r="AJ48" s="48"/>
+      <c r="AK48" s="49"/>
+      <c r="AL48" s="49"/>
+      <c r="AM48" s="49"/>
+      <c r="AN48" s="49"/>
+      <c r="AO48" s="49"/>
+      <c r="AP48" s="49"/>
+      <c r="AQ48" s="4"/>
+      <c r="AR48" s="4"/>
+      <c r="AS48" s="50"/>
+      <c r="AT48" s="48"/>
+      <c r="AU48" s="48"/>
+      <c r="AV48" s="49"/>
+      <c r="AW48" s="49"/>
+      <c r="AX48" s="49"/>
+      <c r="AY48" s="49"/>
+      <c r="AZ48" s="49"/>
+      <c r="BA48" s="49"/>
+      <c r="BB48" s="4"/>
+    </row>
+    <row r="49" spans="29:54" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC49" s="4"/>
+      <c r="AD49" s="4"/>
       <c r="AE49" s="4"/>
       <c r="AF49" s="4"/>
       <c r="AG49" s="4"/>
       <c r="AH49" s="4"/>
-      <c r="AI49" s="4"/>
-      <c r="AJ49" s="4"/>
-      <c r="AK49" s="54"/>
-      <c r="AL49" s="54"/>
-      <c r="AM49" s="55"/>
-      <c r="AN49" s="55"/>
-      <c r="AO49" s="55"/>
-      <c r="AP49" s="55"/>
-      <c r="AQ49" s="55"/>
-      <c r="AR49" s="55"/>
+      <c r="AI49" s="48"/>
+      <c r="AJ49" s="48"/>
+      <c r="AK49" s="49"/>
+      <c r="AL49" s="49"/>
+      <c r="AM49" s="49"/>
+      <c r="AN49" s="49"/>
+      <c r="AO49" s="49"/>
+      <c r="AP49" s="49"/>
+      <c r="AQ49" s="4"/>
+      <c r="AR49" s="4"/>
       <c r="AS49" s="4"/>
-      <c r="AT49" s="4"/>
-      <c r="AU49" s="4"/>
-      <c r="AV49" s="54"/>
-      <c r="AW49" s="54"/>
-      <c r="AX49" s="55"/>
-      <c r="AY49" s="55"/>
-      <c r="AZ49" s="55"/>
-      <c r="BA49" s="55"/>
-      <c r="BB49" s="55"/>
-      <c r="BC49" s="55"/>
-      <c r="BD49" s="4"/>
-    </row>
-    <row r="50" spans="31:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AT49" s="48"/>
+      <c r="AU49" s="48"/>
+      <c r="AV49" s="49"/>
+      <c r="AW49" s="49"/>
+      <c r="AX49" s="49"/>
+      <c r="AY49" s="49"/>
+      <c r="AZ49" s="49"/>
+      <c r="BA49" s="49"/>
+      <c r="BB49" s="4"/>
+    </row>
+    <row r="50" spans="29:54" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC50" s="4"/>
+      <c r="AD50" s="4"/>
       <c r="AE50" s="4"/>
       <c r="AF50" s="4"/>
       <c r="AG50" s="4"/>
       <c r="AH50" s="4"/>
-      <c r="AI50" s="4"/>
-      <c r="AJ50" s="4"/>
-      <c r="AK50" s="54"/>
-      <c r="AL50" s="54"/>
-      <c r="AM50" s="55"/>
-      <c r="AN50" s="55"/>
-      <c r="AO50" s="55"/>
-      <c r="AP50" s="55"/>
-      <c r="AQ50" s="55"/>
-      <c r="AR50" s="55"/>
+      <c r="AI50" s="48"/>
+      <c r="AJ50" s="48"/>
+      <c r="AK50" s="49"/>
+      <c r="AL50" s="49"/>
+      <c r="AM50" s="49"/>
+      <c r="AN50" s="49"/>
+      <c r="AO50" s="49"/>
+      <c r="AP50" s="49"/>
+      <c r="AQ50" s="4"/>
+      <c r="AR50" s="4"/>
       <c r="AS50" s="4"/>
-      <c r="AT50" s="4"/>
-      <c r="AU50" s="4"/>
-      <c r="AV50" s="54"/>
-      <c r="AW50" s="54"/>
-      <c r="AX50" s="55"/>
-      <c r="AY50" s="55"/>
-      <c r="AZ50" s="55"/>
-      <c r="BA50" s="55"/>
-      <c r="BB50" s="55"/>
-      <c r="BC50" s="55"/>
-      <c r="BD50" s="4"/>
-    </row>
-    <row r="51" spans="31:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AT50" s="48"/>
+      <c r="AU50" s="48"/>
+      <c r="AV50" s="49"/>
+      <c r="AW50" s="49"/>
+      <c r="AX50" s="49"/>
+      <c r="AY50" s="49"/>
+      <c r="AZ50" s="49"/>
+      <c r="BA50" s="49"/>
+      <c r="BB50" s="4"/>
+    </row>
+    <row r="51" spans="29:54" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC51" s="4"/>
+      <c r="AD51" s="4"/>
       <c r="AE51" s="4"/>
       <c r="AF51" s="4"/>
       <c r="AG51" s="4"/>
-      <c r="AH51" s="4"/>
-      <c r="AI51" s="4"/>
-      <c r="AJ51" s="54"/>
-      <c r="AK51" s="54"/>
-      <c r="AL51" s="54"/>
-      <c r="AM51" s="55"/>
-      <c r="AN51" s="55"/>
-      <c r="AO51" s="55"/>
-      <c r="AP51" s="55"/>
-      <c r="AQ51" s="55"/>
-      <c r="AR51" s="55"/>
-      <c r="AS51" s="4"/>
-      <c r="AT51" s="4"/>
-      <c r="AU51" s="54"/>
-      <c r="AV51" s="54"/>
-      <c r="AW51" s="54"/>
-      <c r="AX51" s="55"/>
-      <c r="AY51" s="55"/>
-      <c r="AZ51" s="55"/>
-      <c r="BA51" s="55"/>
-      <c r="BB51" s="55"/>
-      <c r="BC51" s="55"/>
-      <c r="BD51" s="4"/>
-    </row>
-    <row r="52" spans="31:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH51" s="48"/>
+      <c r="AI51" s="48"/>
+      <c r="AJ51" s="48"/>
+      <c r="AK51" s="49"/>
+      <c r="AL51" s="49"/>
+      <c r="AM51" s="49"/>
+      <c r="AN51" s="49"/>
+      <c r="AO51" s="49"/>
+      <c r="AP51" s="49"/>
+      <c r="AQ51" s="4"/>
+      <c r="AR51" s="4"/>
+      <c r="AS51" s="48"/>
+      <c r="AT51" s="48"/>
+      <c r="AU51" s="48"/>
+      <c r="AV51" s="49"/>
+      <c r="AW51" s="49"/>
+      <c r="AX51" s="49"/>
+      <c r="AY51" s="49"/>
+      <c r="AZ51" s="49"/>
+      <c r="BA51" s="49"/>
+      <c r="BB51" s="4"/>
+    </row>
+    <row r="52" spans="29:54" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC52" s="4"/>
+      <c r="AD52" s="4"/>
       <c r="AE52" s="4"/>
       <c r="AF52" s="4"/>
       <c r="AG52" s="4"/>
-      <c r="AH52" s="4"/>
-      <c r="AI52" s="4"/>
-      <c r="AJ52" s="56"/>
-      <c r="AK52" s="54"/>
+      <c r="AH52" s="50"/>
+      <c r="AI52" s="48"/>
+      <c r="AJ52" s="4"/>
+      <c r="AK52" s="49"/>
       <c r="AL52" s="4"/>
-      <c r="AM52" s="55"/>
+      <c r="AM52" s="49"/>
       <c r="AN52" s="4"/>
-      <c r="AO52" s="55"/>
+      <c r="AO52" s="49"/>
       <c r="AP52" s="4"/>
-      <c r="AQ52" s="55"/>
+      <c r="AQ52" s="4"/>
       <c r="AR52" s="4"/>
-      <c r="AS52" s="4"/>
-      <c r="AT52" s="4"/>
-      <c r="AU52" s="56"/>
-      <c r="AV52" s="54"/>
+      <c r="AS52" s="50"/>
+      <c r="AT52" s="48"/>
+      <c r="AU52" s="4"/>
+      <c r="AV52" s="49"/>
       <c r="AW52" s="4"/>
-      <c r="AX52" s="55"/>
+      <c r="AX52" s="49"/>
       <c r="AY52" s="4"/>
-      <c r="AZ52" s="55"/>
+      <c r="AZ52" s="49"/>
       <c r="BA52" s="4"/>
-      <c r="BB52" s="55"/>
-      <c r="BC52" s="4"/>
-      <c r="BD52" s="4"/>
-    </row>
-    <row r="53" spans="31:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BB52" s="4"/>
+    </row>
+    <row r="53" spans="29:54" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC53" s="4"/>
+      <c r="AD53" s="4"/>
       <c r="AE53" s="4"/>
       <c r="AF53" s="4"/>
       <c r="AG53" s="4"/>
       <c r="AH53" s="4"/>
-      <c r="AI53" s="4"/>
-      <c r="AJ53" s="4"/>
-      <c r="AK53" s="54"/>
-      <c r="AL53" s="54"/>
-      <c r="AM53" s="55"/>
-      <c r="AN53" s="55"/>
-      <c r="AO53" s="55"/>
-      <c r="AP53" s="55"/>
-      <c r="AQ53" s="55"/>
-      <c r="AR53" s="55"/>
+      <c r="AI53" s="48"/>
+      <c r="AJ53" s="48"/>
+      <c r="AK53" s="49"/>
+      <c r="AL53" s="49"/>
+      <c r="AM53" s="49"/>
+      <c r="AN53" s="49"/>
+      <c r="AO53" s="49"/>
+      <c r="AP53" s="49"/>
+      <c r="AQ53" s="4"/>
+      <c r="AR53" s="4"/>
       <c r="AS53" s="4"/>
-      <c r="AT53" s="4"/>
-      <c r="AU53" s="4"/>
-      <c r="AV53" s="54"/>
-      <c r="AW53" s="54"/>
-      <c r="AX53" s="55"/>
-      <c r="AY53" s="55"/>
-      <c r="AZ53" s="55"/>
-      <c r="BA53" s="55"/>
-      <c r="BB53" s="55"/>
-      <c r="BC53" s="55"/>
-      <c r="BD53" s="4"/>
-    </row>
-    <row r="54" spans="31:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AT53" s="48"/>
+      <c r="AU53" s="48"/>
+      <c r="AV53" s="49"/>
+      <c r="AW53" s="49"/>
+      <c r="AX53" s="49"/>
+      <c r="AY53" s="49"/>
+      <c r="AZ53" s="49"/>
+      <c r="BA53" s="49"/>
+      <c r="BB53" s="4"/>
+    </row>
+    <row r="54" spans="29:54" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC54" s="4"/>
+      <c r="AD54" s="4"/>
       <c r="AE54" s="4"/>
       <c r="AF54" s="4"/>
       <c r="AG54" s="4"/>
@@ -4160,10 +4337,10 @@
       <c r="AZ54" s="4"/>
       <c r="BA54" s="4"/>
       <c r="BB54" s="4"/>
-      <c r="BC54" s="4"/>
-      <c r="BD54" s="4"/>
-    </row>
-    <row r="55" spans="31:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="29:54" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC55" s="4"/>
+      <c r="AD55" s="4"/>
       <c r="AE55" s="4"/>
       <c r="AF55" s="4"/>
       <c r="AG55" s="4"/>
@@ -4188,10 +4365,10 @@
       <c r="AZ55" s="4"/>
       <c r="BA55" s="4"/>
       <c r="BB55" s="4"/>
-      <c r="BC55" s="4"/>
-      <c r="BD55" s="4"/>
-    </row>
-    <row r="56" spans="31:56" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="29:54" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC56" s="4"/>
+      <c r="AD56" s="4"/>
       <c r="AE56" s="4"/>
       <c r="AF56" s="4"/>
       <c r="AG56" s="4"/>
@@ -4216,31 +4393,30 @@
       <c r="AZ56" s="4"/>
       <c r="BA56" s="4"/>
       <c r="BB56" s="4"/>
-      <c r="BC56" s="4"/>
-      <c r="BD56" s="4"/>
-    </row>
-    <row r="57" spans="31:56" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" spans="31:56" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="31:56" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="31:56" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" spans="31:56" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" spans="31:56" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" spans="31:56" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="31:56" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="57" spans="29:54" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="29:54" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="29:54" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="29:54" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="29:54" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="29:54" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="29:54" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="29:54" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="65" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
     <mergeCell ref="A25:X25"/>
     <mergeCell ref="T3:U3"/>
     <mergeCell ref="T14:U14"/>
     <mergeCell ref="A22:X22"/>
     <mergeCell ref="A23:X23"/>
     <mergeCell ref="A24:X24"/>
+    <mergeCell ref="S5:W6"/>
+    <mergeCell ref="M33:O33"/>
+    <mergeCell ref="P33:R33"/>
+    <mergeCell ref="S33:U33"/>
     <mergeCell ref="A26:U26"/>
     <mergeCell ref="A28:L28"/>
-    <mergeCell ref="M29:O29"/>
-    <mergeCell ref="P29:R29"/>
-    <mergeCell ref="S29:U29"/>
   </mergeCells>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0" footer="0"/>
   <pageSetup scale="43" orientation="landscape" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>